<commit_message>
tweaks to Excel survey template
</commit_message>
<xml_diff>
--- a/inst/snow_survey/SnowSurveyTemplate.xlsx
+++ b/inst/snow_survey/SnowSurveyTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estewart\Documents\R\Projects\YGwater\inst\snow_survey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\snow_survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F6BE4C-2364-48DB-A927-59414433945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C29627D-AB32-4213-B07F-5F126E555A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="0" windowWidth="18105" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -190,15 +190,6 @@
     <t>QA/QC-ed</t>
   </si>
   <si>
-    <t>Tare</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>SWE</t>
-  </si>
-  <si>
     <r>
       <t>Weather at time of sampling</t>
     </r>
@@ -391,6 +382,15 @@
   </si>
   <si>
     <t>no sample</t>
+  </si>
+  <si>
+    <t>SWE (cm)</t>
+  </si>
+  <si>
+    <t>Weight (cm)</t>
+  </si>
+  <si>
+    <t>Tare (cm)</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1188,9 +1188,6 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -1346,6 +1343,15 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1368,22 +1374,25 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1422,6 +1431,15 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1455,28 +1473,28 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1525,6 +1543,10 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1552,6 +1574,9 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1560,6 +1585,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1643,289 +1671,15 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="20" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="67">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2294,6 +2048,249 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3621,21 +3618,15 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="2" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.140625" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" customWidth="1"/>
     <col min="13" max="13" width="5.42578125" customWidth="1"/>
@@ -3658,189 +3649,189 @@
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="154" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="146"/>
-      <c r="J2" s="146"/>
-      <c r="K2" s="146"/>
-      <c r="L2" s="147"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="155"/>
+      <c r="K2" s="155"/>
+      <c r="L2" s="156"/>
       <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
-      <c r="B3" s="148"/>
-      <c r="C3" s="149"/>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149"/>
-      <c r="F3" s="149"/>
-      <c r="G3" s="149"/>
-      <c r="H3" s="149"/>
-      <c r="I3" s="149"/>
-      <c r="J3" s="149"/>
-      <c r="K3" s="149"/>
-      <c r="L3" s="150"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
+      <c r="L3" s="159"/>
       <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="164"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="165"/>
-      <c r="H4" s="165"/>
-      <c r="I4" s="165"/>
-      <c r="J4" s="99" t="s">
-        <v>75</v>
-      </c>
-      <c r="K4" s="100"/>
-      <c r="L4" s="101"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="174"/>
+      <c r="E4" s="174"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="174"/>
+      <c r="H4" s="174"/>
+      <c r="I4" s="174"/>
+      <c r="J4" s="102" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="103"/>
+      <c r="L4" s="104"/>
       <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="166"/>
-      <c r="E5" s="166"/>
-      <c r="F5" s="166"/>
-      <c r="G5" s="166"/>
-      <c r="H5" s="166"/>
-      <c r="I5" s="166"/>
-      <c r="J5" s="151" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="152"/>
-      <c r="L5" s="153"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="175"/>
+      <c r="E5" s="175"/>
+      <c r="F5" s="175"/>
+      <c r="G5" s="175"/>
+      <c r="H5" s="175"/>
+      <c r="I5" s="175"/>
+      <c r="J5" s="160" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="161"/>
+      <c r="L5" s="162"/>
       <c r="M5" s="15"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="123" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="167"/>
-      <c r="E6" s="167"/>
-      <c r="F6" s="167"/>
-      <c r="G6" s="167"/>
-      <c r="H6" s="167"/>
-      <c r="I6" s="167"/>
-      <c r="J6" s="154" t="s">
-        <v>62</v>
-      </c>
-      <c r="K6" s="155"/>
-      <c r="L6" s="156"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="176"/>
+      <c r="H6" s="176"/>
+      <c r="I6" s="176"/>
+      <c r="J6" s="163" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="164"/>
+      <c r="L6" s="165"/>
       <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="111" t="s">
+      <c r="B7" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="112"/>
-      <c r="D7" s="172"/>
-      <c r="E7" s="172"/>
-      <c r="F7" s="172"/>
-      <c r="G7" s="172"/>
-      <c r="H7" s="172"/>
-      <c r="I7" s="172"/>
-      <c r="J7" s="157" t="s">
-        <v>79</v>
-      </c>
-      <c r="K7" s="158"/>
-      <c r="L7" s="159"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="166" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="167"/>
+      <c r="L7" s="168"/>
       <c r="M7" s="15"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="111" t="s">
+      <c r="B8" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="112"/>
-      <c r="D8" s="171"/>
-      <c r="E8" s="171"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="171"/>
-      <c r="H8" s="171"/>
-      <c r="I8" s="171"/>
-      <c r="J8" s="168" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" s="169"/>
-      <c r="L8" s="170"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="180"/>
+      <c r="G8" s="180"/>
+      <c r="H8" s="180"/>
+      <c r="I8" s="180"/>
+      <c r="J8" s="177" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" s="178"/>
+      <c r="L8" s="179"/>
       <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="112"/>
-      <c r="D9" s="119" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="160" t="s">
+      <c r="C9" s="124"/>
+      <c r="D9" s="125" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="126"/>
+      <c r="J9" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="161"/>
-      <c r="L9" s="162"/>
+      <c r="K9" s="170"/>
+      <c r="L9" s="171"/>
       <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="111" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="121" t="s">
+      <c r="B10" s="123" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="124"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="122"/>
-      <c r="L10" s="123"/>
+      <c r="K10" s="128"/>
+      <c r="L10" s="129"/>
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
-      <c r="B11" s="127" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="128"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="124" t="s">
+      <c r="B11" s="133" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="134"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="125"/>
-      <c r="L11" s="126"/>
+      <c r="K11" s="131"/>
+      <c r="L11" s="132"/>
       <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
@@ -3855,13 +3846,13 @@
         <v>4</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>6</v>
@@ -3870,19 +3861,19 @@
         <v>29</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K12" s="26" t="s">
         <v>9</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M12" s="15"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
-      <c r="B13" s="44">
+      <c r="B13" s="43">
         <v>1</v>
       </c>
       <c r="C13" s="29"/>
@@ -3897,18 +3888,18 @@
         <f t="shared" ref="H13:H22" si="0">IFERROR(IF($D$9="standard", (G13/C13)*100, ""), "")</f>
         <v/>
       </c>
-      <c r="I13" s="45" t="str">
+      <c r="I13" s="44" t="str">
         <f>IFERROR(D13/C13*100, "")</f>
         <v/>
       </c>
-      <c r="J13" s="43"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="47"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="46"/>
       <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" s="44">
+      <c r="B14" s="43">
         <v>2</v>
       </c>
       <c r="C14" s="29"/>
@@ -3920,21 +3911,21 @@
         <v/>
       </c>
       <c r="H14" s="31" t="str">
-        <f t="shared" si="0"/>
+        <f>IFERROR(IF($D$9="standard", (G14/C14)*100, ""), "")</f>
         <v/>
       </c>
-      <c r="I14" s="45" t="str">
+      <c r="I14" s="44" t="str">
         <f t="shared" ref="I14:I22" si="2">IFERROR(D14/C14*100, "")</f>
         <v/>
       </c>
-      <c r="J14" s="48"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="49"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="48"/>
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
-      <c r="B15" s="44">
+      <c r="B15" s="43">
         <v>3</v>
       </c>
       <c r="C15" s="29"/>
@@ -3949,18 +3940,18 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I15" s="45" t="str">
+      <c r="I15" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J15" s="43"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="49"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="48"/>
       <c r="M15" s="16"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
-      <c r="B16" s="44">
+      <c r="B16" s="43">
         <v>4</v>
       </c>
       <c r="C16" s="29"/>
@@ -3975,19 +3966,19 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I16" s="45" t="str">
+      <c r="I16" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J16" s="43"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="49"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="48"/>
       <c r="M16" s="15"/>
       <c r="S16" s="2"/>
     </row>
     <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
-      <c r="B17" s="44">
+      <c r="B17" s="43">
         <v>5</v>
       </c>
       <c r="C17" s="29"/>
@@ -4002,18 +3993,18 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I17" s="45" t="str">
+      <c r="I17" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J17" s="43"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="49"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="48"/>
       <c r="M17" s="15"/>
     </row>
     <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
-      <c r="B18" s="44">
+      <c r="B18" s="43">
         <v>6</v>
       </c>
       <c r="C18" s="29"/>
@@ -4028,18 +4019,18 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I18" s="45" t="str">
+      <c r="I18" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J18" s="43"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="49"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="48"/>
       <c r="M18" s="15"/>
     </row>
     <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
-      <c r="B19" s="44">
+      <c r="B19" s="43">
         <v>7</v>
       </c>
       <c r="C19" s="29"/>
@@ -4054,18 +4045,18 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I19" s="45" t="str">
+      <c r="I19" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J19" s="43"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="49"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="48"/>
       <c r="M19" s="15"/>
     </row>
     <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
-      <c r="B20" s="44">
+      <c r="B20" s="43">
         <v>8</v>
       </c>
       <c r="C20" s="29"/>
@@ -4080,18 +4071,18 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I20" s="45" t="str">
+      <c r="I20" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J20" s="43"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="49"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="48"/>
       <c r="M20" s="15"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
-      <c r="B21" s="44">
+      <c r="B21" s="43">
         <v>9</v>
       </c>
       <c r="C21" s="29"/>
@@ -4106,18 +4097,18 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I21" s="45" t="str">
+      <c r="I21" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J21" s="43"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="49"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="48"/>
       <c r="M21" s="15"/>
     </row>
     <row r="22" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
-      <c r="B22" s="44">
+      <c r="B22" s="43">
         <v>10</v>
       </c>
       <c r="C22" s="29"/>
@@ -4132,89 +4123,89 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I22" s="45" t="str">
+      <c r="I22" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J22" s="33"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="51"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="50"/>
       <c r="M22" s="15"/>
     </row>
     <row r="23" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35" t="str">
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34" t="str">
         <f>IF(OR(ISBLANK(E23),ISBLANK(F23)),"",IF($D$9="bulk",F23-E23,""))</f>
         <v/>
       </c>
-      <c r="H23" s="36" t="str">
+      <c r="H23" s="35" t="str">
         <f>IFERROR(IF($D$9="bulk", G23/(SUM(C13:C22))*100, ""), "")</f>
         <v/>
       </c>
       <c r="I23" s="22"/>
       <c r="J23" s="22"/>
-      <c r="K23" s="129" t="s">
-        <v>61</v>
-      </c>
-      <c r="L23" s="131"/>
+      <c r="K23" s="135" t="s">
+        <v>58</v>
+      </c>
+      <c r="L23" s="137"/>
       <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="37">
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="36" t="str">
         <f>IF($D$9="standard",SUMIFS(G13:G22, K13:K22, ""), "")</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="39"/>
+        <v/>
+      </c>
+      <c r="H24" s="38"/>
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
-      <c r="K24" s="130"/>
-      <c r="L24" s="132"/>
+      <c r="K24" s="136"/>
+      <c r="L24" s="138"/>
       <c r="M24" s="15"/>
     </row>
     <row r="25" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="40" t="str">
+      <c r="C25" s="39" t="str">
         <f>IFERROR(AVERAGEIFS(C13:C22, K13:K22, ""), "")</f>
         <v/>
       </c>
-      <c r="D25" s="40" t="str">
+      <c r="D25" s="39" t="str">
         <f>IFERROR(AVERAGEIFS(D13:D22, K13:K22, ""), "")</f>
         <v/>
       </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="40" t="str">
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="39" t="str">
         <f>IFERROR(IF($D$9="Standard", AVERAGEIFS(G13:G22, K13:K22, ""), IF(D9="Bulk",G23/COUNT(D13:D22),"")),"")</f>
         <v/>
       </c>
-      <c r="H25" s="42" t="str">
+      <c r="H25" s="41" t="str">
         <f>IFERROR(IF($D$9="standard", AVERAGEIFS(H13:H22, K13:K22, ""), IF($D$9="Bulk",H23,"")), "")</f>
         <v/>
       </c>
       <c r="I25" s="22"/>
       <c r="J25" s="22"/>
-      <c r="K25" s="55" t="s">
+      <c r="K25" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="L25" s="56"/>
+      <c r="L25" s="55"/>
       <c r="M25" s="17"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
@@ -4224,13 +4215,13 @@
     </row>
     <row r="26" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
@@ -4244,19 +4235,19 @@
     </row>
     <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
-      <c r="B27" s="86" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="88"/>
+      <c r="B27" s="105" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="106"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="107"/>
       <c r="J27" s="22"/>
-      <c r="K27" s="60"/>
-      <c r="L27" s="60"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
       <c r="M27" s="17"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
@@ -4266,19 +4257,19 @@
     </row>
     <row r="28" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
-      <c r="B28" s="138" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="139"/>
-      <c r="D28" s="139"/>
-      <c r="E28" s="139"/>
-      <c r="F28" s="139"/>
-      <c r="G28" s="139"/>
-      <c r="H28" s="140"/>
+      <c r="B28" s="145" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="147"/>
       <c r="I28" s="28"/>
       <c r="J28" s="22"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="60"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="59"/>
       <c r="M28" s="17"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
@@ -4288,25 +4279,25 @@
     </row>
     <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="63" t="s">
+      <c r="C29" s="61"/>
+      <c r="D29" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63" t="s">
+      <c r="E29" s="61"/>
+      <c r="F29" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="62"/>
-      <c r="H29" s="63" t="s">
+      <c r="G29" s="61"/>
+      <c r="H29" s="62" t="s">
         <v>16</v>
       </c>
       <c r="I29" s="28"/>
       <c r="J29" s="22"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="60"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="59"/>
       <c r="M29" s="17"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
@@ -4316,25 +4307,25 @@
     </row>
     <row r="30" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15"/>
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="66" t="s">
+      <c r="C30" s="64"/>
+      <c r="D30" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="66" t="s">
+      <c r="E30" s="64"/>
+      <c r="F30" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="65"/>
-      <c r="H30" s="66" t="s">
+      <c r="G30" s="64"/>
+      <c r="H30" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="67"/>
+      <c r="I30" s="66"/>
       <c r="J30" s="22"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="60"/>
+      <c r="K30" s="59"/>
+      <c r="L30" s="59"/>
       <c r="M30" s="17"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
@@ -4344,19 +4335,19 @@
     </row>
     <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
-      <c r="B31" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="87"/>
-      <c r="I31" s="88"/>
+      <c r="B31" s="105" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="106"/>
+      <c r="I31" s="107"/>
       <c r="J31" s="22"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="60"/>
+      <c r="K31" s="59"/>
+      <c r="L31" s="59"/>
       <c r="M31" s="17"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
@@ -4366,15 +4357,15 @@
     </row>
     <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
-      <c r="B32" s="113" t="s">
+      <c r="B32" s="117" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="114"/>
-      <c r="D32" s="114"/>
-      <c r="E32" s="114"/>
-      <c r="F32" s="114"/>
-      <c r="G32" s="114"/>
-      <c r="H32" s="115"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="118"/>
+      <c r="H32" s="119"/>
       <c r="I32" s="28"/>
       <c r="J32" s="22"/>
       <c r="K32" s="22"/>
@@ -4388,15 +4379,15 @@
     </row>
     <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
-      <c r="B33" s="113" t="s">
+      <c r="B33" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="114"/>
-      <c r="D33" s="114"/>
-      <c r="E33" s="114"/>
-      <c r="F33" s="114"/>
-      <c r="G33" s="114"/>
-      <c r="H33" s="115"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="119"/>
       <c r="I33" s="28"/>
       <c r="J33" s="22"/>
       <c r="K33" s="22"/>
@@ -4410,15 +4401,15 @@
     </row>
     <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
-      <c r="B34" s="113" t="s">
+      <c r="B34" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="114"/>
-      <c r="D34" s="114"/>
-      <c r="E34" s="114"/>
-      <c r="F34" s="114"/>
-      <c r="G34" s="114"/>
-      <c r="H34" s="115"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="119"/>
       <c r="I34" s="28"/>
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
@@ -4432,15 +4423,15 @@
     </row>
     <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
-      <c r="B35" s="113" t="s">
+      <c r="B35" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="114"/>
-      <c r="D35" s="114"/>
-      <c r="E35" s="114"/>
-      <c r="F35" s="114"/>
-      <c r="G35" s="114"/>
-      <c r="H35" s="115"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="119"/>
       <c r="I35" s="28"/>
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
@@ -4454,17 +4445,17 @@
     </row>
     <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="116" t="s">
+      <c r="B36" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="117"/>
-      <c r="D36" s="117"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="118" t="s">
+      <c r="C36" s="121"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="114"/>
-      <c r="H36" s="115"/>
+      <c r="G36" s="118"/>
+      <c r="H36" s="119"/>
       <c r="I36" s="28"/>
       <c r="J36" s="22"/>
       <c r="K36" s="22"/>
@@ -4478,18 +4469,18 @@
     </row>
     <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
-      <c r="B37" s="136" t="s">
+      <c r="B37" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="137"/>
-      <c r="D37" s="137"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="137" t="s">
+      <c r="C37" s="144"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="144" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="137"/>
-      <c r="H37" s="137"/>
-      <c r="I37" s="69"/>
+      <c r="G37" s="144"/>
+      <c r="H37" s="144"/>
+      <c r="I37" s="68"/>
       <c r="J37" s="22"/>
       <c r="K37" s="22"/>
       <c r="L37" s="22"/>
@@ -4502,18 +4493,18 @@
     </row>
     <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
-      <c r="B38" s="136" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="137"/>
-      <c r="D38" s="137"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="141" t="s">
-        <v>85</v>
-      </c>
-      <c r="G38" s="89"/>
-      <c r="H38" s="80"/>
-      <c r="I38" s="71"/>
+      <c r="B38" s="143" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="144"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="148" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38" s="149"/>
+      <c r="H38" s="82"/>
+      <c r="I38" s="70"/>
       <c r="J38" s="22"/>
       <c r="K38" s="22"/>
       <c r="L38" s="22"/>
@@ -4526,16 +4517,16 @@
     </row>
     <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
-      <c r="B39" s="108" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" s="109"/>
-      <c r="D39" s="109"/>
-      <c r="E39" s="109"/>
-      <c r="F39" s="109"/>
-      <c r="G39" s="109"/>
-      <c r="H39" s="109"/>
-      <c r="I39" s="110"/>
+      <c r="B39" s="114" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="115"/>
+      <c r="D39" s="115"/>
+      <c r="E39" s="115"/>
+      <c r="F39" s="115"/>
+      <c r="G39" s="115"/>
+      <c r="H39" s="115"/>
+      <c r="I39" s="116"/>
       <c r="J39" s="22"/>
       <c r="K39" s="22"/>
       <c r="L39" s="22"/>
@@ -4548,14 +4539,14 @@
     </row>
     <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
-      <c r="B40" s="102"/>
-      <c r="C40" s="103"/>
-      <c r="D40" s="103"/>
-      <c r="E40" s="103"/>
-      <c r="F40" s="103"/>
-      <c r="G40" s="103"/>
-      <c r="H40" s="103"/>
-      <c r="I40" s="104"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="109"/>
+      <c r="E40" s="109"/>
+      <c r="F40" s="109"/>
+      <c r="G40" s="109"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="110"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
@@ -4568,14 +4559,14 @@
     </row>
     <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
-      <c r="B41" s="102"/>
-      <c r="C41" s="103"/>
-      <c r="D41" s="103"/>
-      <c r="E41" s="103"/>
-      <c r="F41" s="103"/>
-      <c r="G41" s="103"/>
-      <c r="H41" s="103"/>
-      <c r="I41" s="104"/>
+      <c r="B41" s="108"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="109"/>
+      <c r="F41" s="109"/>
+      <c r="G41" s="109"/>
+      <c r="H41" s="109"/>
+      <c r="I41" s="110"/>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
       <c r="L41" s="17"/>
@@ -4588,14 +4579,14 @@
     </row>
     <row r="42" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
-      <c r="B42" s="105"/>
-      <c r="C42" s="106"/>
-      <c r="D42" s="106"/>
-      <c r="E42" s="106"/>
-      <c r="F42" s="106"/>
-      <c r="G42" s="106"/>
-      <c r="H42" s="106"/>
-      <c r="I42" s="107"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="112"/>
+      <c r="G42" s="112"/>
+      <c r="H42" s="112"/>
+      <c r="I42" s="113"/>
       <c r="J42" s="17"/>
       <c r="K42" s="17"/>
       <c r="L42" s="17"/>
@@ -4608,16 +4599,16 @@
     </row>
     <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
-      <c r="B43" s="142" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="143"/>
-      <c r="D43" s="143"/>
-      <c r="E43" s="143"/>
-      <c r="F43" s="143"/>
-      <c r="G43" s="143"/>
-      <c r="H43" s="143"/>
-      <c r="I43" s="144"/>
+      <c r="B43" s="150" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="151"/>
+      <c r="D43" s="151"/>
+      <c r="E43" s="151"/>
+      <c r="F43" s="151"/>
+      <c r="G43" s="151"/>
+      <c r="H43" s="151"/>
+      <c r="I43" s="152"/>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
@@ -4630,15 +4621,15 @@
     </row>
     <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
-      <c r="B44" s="113" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="114"/>
-      <c r="D44" s="114"/>
-      <c r="E44" s="114"/>
-      <c r="F44" s="114"/>
-      <c r="G44" s="114"/>
-      <c r="H44" s="115"/>
+      <c r="B44" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="118"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="118"/>
+      <c r="F44" s="118"/>
+      <c r="G44" s="118"/>
+      <c r="H44" s="119"/>
       <c r="I44" s="28"/>
       <c r="J44" s="17"/>
       <c r="K44" s="17"/>
@@ -4652,15 +4643,15 @@
     </row>
     <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
-      <c r="B45" s="113" t="s">
+      <c r="B45" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="114"/>
-      <c r="D45" s="114"/>
-      <c r="E45" s="114"/>
-      <c r="F45" s="114"/>
-      <c r="G45" s="114"/>
-      <c r="H45" s="115"/>
+      <c r="C45" s="118"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="118"/>
+      <c r="F45" s="118"/>
+      <c r="G45" s="118"/>
+      <c r="H45" s="119"/>
       <c r="I45" s="28"/>
       <c r="J45" s="17"/>
       <c r="K45" s="17"/>
@@ -4674,15 +4665,15 @@
     </row>
     <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
-      <c r="B46" s="113" t="s">
+      <c r="B46" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="114"/>
-      <c r="D46" s="114"/>
-      <c r="E46" s="114"/>
-      <c r="F46" s="114"/>
-      <c r="G46" s="114"/>
-      <c r="H46" s="115"/>
+      <c r="C46" s="118"/>
+      <c r="D46" s="118"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118"/>
+      <c r="G46" s="118"/>
+      <c r="H46" s="119"/>
       <c r="I46" s="28"/>
       <c r="J46" s="17"/>
       <c r="K46" s="17"/>
@@ -4696,16 +4687,16 @@
     </row>
     <row r="47" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15"/>
-      <c r="B47" s="133" t="s">
+      <c r="B47" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="134"/>
-      <c r="D47" s="134"/>
-      <c r="E47" s="134"/>
-      <c r="F47" s="134"/>
-      <c r="G47" s="134"/>
-      <c r="H47" s="135"/>
-      <c r="I47" s="69"/>
+      <c r="C47" s="141"/>
+      <c r="D47" s="141"/>
+      <c r="E47" s="141"/>
+      <c r="F47" s="141"/>
+      <c r="G47" s="141"/>
+      <c r="H47" s="142"/>
+      <c r="I47" s="68"/>
       <c r="J47" s="17"/>
       <c r="K47" s="17"/>
       <c r="L47" s="17"/>
@@ -4718,16 +4709,16 @@
     </row>
     <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
-      <c r="B48" s="86" t="s">
-        <v>72</v>
-      </c>
-      <c r="C48" s="87"/>
-      <c r="D48" s="87"/>
-      <c r="E48" s="87"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="87"/>
-      <c r="H48" s="87"/>
-      <c r="I48" s="88"/>
+      <c r="B48" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="106"/>
+      <c r="D48" s="106"/>
+      <c r="E48" s="106"/>
+      <c r="F48" s="106"/>
+      <c r="G48" s="106"/>
+      <c r="H48" s="106"/>
+      <c r="I48" s="107"/>
       <c r="J48" s="17"/>
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
@@ -4735,15 +4726,15 @@
     </row>
     <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
-      <c r="B49" s="84" t="s">
-        <v>73</v>
-      </c>
-      <c r="C49" s="85"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="85"/>
+      <c r="B49" s="86" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="87"/>
+      <c r="D49" s="87"/>
+      <c r="E49" s="87"/>
+      <c r="F49" s="87"/>
+      <c r="G49" s="87"/>
+      <c r="H49" s="87"/>
       <c r="I49" s="28"/>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
@@ -4752,15 +4743,15 @@
     </row>
     <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
-      <c r="B50" s="84" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="85"/>
-      <c r="D50" s="85"/>
-      <c r="E50" s="85"/>
-      <c r="F50" s="85"/>
-      <c r="G50" s="85"/>
-      <c r="H50" s="85"/>
+      <c r="B50" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="87"/>
+      <c r="D50" s="87"/>
+      <c r="E50" s="87"/>
+      <c r="F50" s="87"/>
+      <c r="G50" s="87"/>
+      <c r="H50" s="87"/>
       <c r="I50" s="28"/>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
@@ -4769,15 +4760,15 @@
     </row>
     <row r="51" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
-      <c r="B51" s="84" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="85"/>
-      <c r="D51" s="85"/>
-      <c r="E51" s="85"/>
-      <c r="F51" s="85"/>
-      <c r="G51" s="85"/>
-      <c r="H51" s="85"/>
+      <c r="B51" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="87"/>
+      <c r="D51" s="87"/>
+      <c r="E51" s="87"/>
+      <c r="F51" s="87"/>
+      <c r="G51" s="87"/>
+      <c r="H51" s="87"/>
       <c r="I51" s="28"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
@@ -4786,16 +4777,16 @@
     </row>
     <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
-      <c r="B52" s="99" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" s="100"/>
-      <c r="D52" s="100"/>
-      <c r="E52" s="100"/>
-      <c r="F52" s="100"/>
-      <c r="G52" s="100"/>
-      <c r="H52" s="100"/>
-      <c r="I52" s="101"/>
+      <c r="B52" s="102" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="103"/>
+      <c r="D52" s="103"/>
+      <c r="E52" s="103"/>
+      <c r="F52" s="103"/>
+      <c r="G52" s="103"/>
+      <c r="H52" s="103"/>
+      <c r="I52" s="104"/>
       <c r="J52" s="17"/>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
@@ -4803,14 +4794,14 @@
     </row>
     <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
-      <c r="B53" s="93"/>
-      <c r="C53" s="94"/>
-      <c r="D53" s="94"/>
-      <c r="E53" s="94"/>
-      <c r="F53" s="94"/>
-      <c r="G53" s="94"/>
-      <c r="H53" s="94"/>
-      <c r="I53" s="95"/>
+      <c r="B53" s="96"/>
+      <c r="C53" s="97"/>
+      <c r="D53" s="97"/>
+      <c r="E53" s="97"/>
+      <c r="F53" s="97"/>
+      <c r="G53" s="97"/>
+      <c r="H53" s="97"/>
+      <c r="I53" s="98"/>
       <c r="J53" s="17"/>
       <c r="K53" s="17"/>
       <c r="L53" s="17"/>
@@ -4818,14 +4809,14 @@
     </row>
     <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
-      <c r="B54" s="93"/>
-      <c r="C54" s="94"/>
-      <c r="D54" s="94"/>
-      <c r="E54" s="94"/>
-      <c r="F54" s="94"/>
-      <c r="G54" s="94"/>
-      <c r="H54" s="94"/>
-      <c r="I54" s="95"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="97"/>
+      <c r="D54" s="97"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="97"/>
+      <c r="G54" s="97"/>
+      <c r="H54" s="97"/>
+      <c r="I54" s="98"/>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
@@ -4833,14 +4824,14 @@
     </row>
     <row r="55" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
-      <c r="B55" s="96"/>
-      <c r="C55" s="97"/>
-      <c r="D55" s="97"/>
-      <c r="E55" s="97"/>
-      <c r="F55" s="97"/>
-      <c r="G55" s="97"/>
-      <c r="H55" s="97"/>
-      <c r="I55" s="98"/>
+      <c r="B55" s="99"/>
+      <c r="C55" s="100"/>
+      <c r="D55" s="100"/>
+      <c r="E55" s="100"/>
+      <c r="F55" s="100"/>
+      <c r="G55" s="100"/>
+      <c r="H55" s="100"/>
+      <c r="I55" s="101"/>
       <c r="J55" s="17"/>
       <c r="K55" s="17"/>
       <c r="L55" s="17"/>
@@ -4863,11 +4854,11 @@
     </row>
     <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
-      <c r="B57" s="174" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" s="175"/>
-      <c r="D57" s="176"/>
+      <c r="B57" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="89"/>
+      <c r="D57" s="90"/>
       <c r="E57" s="24"/>
       <c r="F57" s="24"/>
       <c r="G57" s="24"/>
@@ -4880,11 +4871,11 @@
     </row>
     <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
-      <c r="B58" s="78" t="s">
-        <v>69</v>
-      </c>
-      <c r="C58" s="77"/>
-      <c r="D58" s="180" t="s">
+      <c r="B58" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="76"/>
+      <c r="D58" s="78" t="s">
         <v>39</v>
       </c>
       <c r="E58" s="24"/>
@@ -4899,11 +4890,11 @@
     </row>
     <row r="59" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="15"/>
-      <c r="B59" s="177" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" s="179"/>
-      <c r="D59" s="181" t="s">
+      <c r="B59" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59" s="92"/>
+      <c r="D59" s="79" t="s">
         <v>38</v>
       </c>
       <c r="E59" s="24"/>
@@ -4918,12 +4909,12 @@
     </row>
     <row r="60" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
-      <c r="B60" s="90" t="s">
-        <v>88</v>
-      </c>
-      <c r="C60" s="91"/>
-      <c r="D60" s="182" t="s">
-        <v>89</v>
+      <c r="B60" s="94" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="153"/>
+      <c r="D60" s="80" t="s">
+        <v>86</v>
       </c>
       <c r="E60" s="24"/>
       <c r="F60" s="24"/>
@@ -4937,11 +4928,11 @@
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
-      <c r="B61" s="177" t="s">
-        <v>65</v>
-      </c>
-      <c r="C61" s="178"/>
-      <c r="D61" s="74">
+      <c r="B61" s="91" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="93"/>
+      <c r="D61" s="73">
         <v>4</v>
       </c>
       <c r="E61" s="24"/>
@@ -4956,11 +4947,11 @@
     </row>
     <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="15"/>
-      <c r="B62" s="90" t="s">
-        <v>66</v>
-      </c>
-      <c r="C62" s="92"/>
-      <c r="D62" s="73">
+      <c r="B62" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" s="95"/>
+      <c r="D62" s="72">
         <v>5</v>
       </c>
       <c r="E62" s="24"/>
@@ -4975,11 +4966,11 @@
     </row>
     <row r="63" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
-      <c r="B63" s="79" t="s">
-        <v>67</v>
-      </c>
-      <c r="C63" s="80"/>
-      <c r="D63" s="72">
+      <c r="B63" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" s="82"/>
+      <c r="D63" s="71">
         <v>50</v>
       </c>
       <c r="E63" s="24"/>
@@ -4994,11 +4985,11 @@
     </row>
     <row r="64" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="15"/>
-      <c r="B64" s="82" t="s">
-        <v>68</v>
-      </c>
-      <c r="C64" s="83"/>
-      <c r="D64" s="75">
+      <c r="B64" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="85"/>
+      <c r="D64" s="74">
         <v>66</v>
       </c>
       <c r="E64" s="24"/>
@@ -5096,7 +5087,6 @@
       <c r="B78" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="p4Z1y41EWhKXxqpUpGaD/Uyiwm0NuWd8PXtRmG+8JL+ppYQxZKpKz6/jp4idVlAESd+X9BSLv7MyEO+vTUGLRA==" saltValue="Ezrpf1HSnzI06e8atzOeBg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="60">
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B2:L3"/>
@@ -5127,6 +5117,13 @@
     <mergeCell ref="F37:H37"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:I9"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="B27:I27"/>
@@ -5135,14 +5132,6 @@
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="D11:I11"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:I9"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="D10:I10"/>
     <mergeCell ref="B64:C64"/>
@@ -5158,103 +5147,104 @@
     <mergeCell ref="B51:H51"/>
     <mergeCell ref="B40:I42"/>
     <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B34:H34"/>
   </mergeCells>
-  <conditionalFormatting sqref="C23:H23">
-    <cfRule type="expression" dxfId="1" priority="1641">
-      <formula>$D$9="standard"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="C13:H22">
+    <cfRule type="expression" dxfId="66" priority="2" stopIfTrue="1">
       <formula>$D$9="no sample"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C23:H23">
+    <cfRule type="expression" dxfId="65" priority="1">
+      <formula>$D$9="no sample"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="1641">
+      <formula>$D$9="standard"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D7:I7">
-    <cfRule type="expression" dxfId="23" priority="1624">
+    <cfRule type="expression" dxfId="63" priority="1624">
       <formula>ISBLANK($D$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="1625">
+    <cfRule type="expression" dxfId="62" priority="1625">
       <formula>OR(D7 &gt; D6 + 6, D7 &lt; D6 - 6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:F23">
-    <cfRule type="expression" dxfId="21" priority="1642">
+    <cfRule type="expression" dxfId="61" priority="1642">
       <formula>$D$9="bulk"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13:H22">
-    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="3" stopIfTrue="1">
       <formula>$D$9="bulk"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13:I22 C13:D22">
-    <cfRule type="expression" dxfId="19" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="6" stopIfTrue="1">
       <formula>NOT(ISBLANK($K13))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:G22">
-    <cfRule type="cellIs" dxfId="18" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="15" operator="greaterThan">
       <formula>($H$25+$D$62)*$C13/100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="16" operator="lessThan">
       <formula>($H$25-$D$62)*$C13/100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="56" priority="17" operator="lessThanOrEqual">
       <formula>($H$25-$D$61)*$C13/100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="18" operator="greaterThanOrEqual">
       <formula>($H$25+$D$61)*$C13/100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
-    <cfRule type="expression" dxfId="14" priority="1637">
+    <cfRule type="expression" dxfId="54" priority="1637">
       <formula>$D$9="standard"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:H22">
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="5" stopIfTrue="1">
       <formula>ISBLANK($F13)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:H23">
-    <cfRule type="expression" dxfId="12" priority="1500">
+    <cfRule type="expression" dxfId="52" priority="1500">
       <formula>$D$9="bulk"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:I22">
-    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="4" stopIfTrue="1">
       <formula>ISBLANK($C13)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H22">
-    <cfRule type="containsBlanks" dxfId="10" priority="7">
+    <cfRule type="containsBlanks" dxfId="50" priority="7">
       <formula>LEN(TRIM(H13))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="8" operator="lessThan">
       <formula>$H$25-$D$62</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="9" operator="greaterThan">
       <formula>$H$25+$D$62</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="47" priority="10" operator="greaterThanOrEqual">
       <formula>$H$25+$D$61</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="46" priority="11" operator="lessThanOrEqual">
       <formula>$H$25-$D$61</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:I22">
-    <cfRule type="cellIs" dxfId="5" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="12" operator="greaterThan">
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="13" operator="lessThan">
       <formula>$D$63</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="14" operator="lessThan">
       <formula>$D$64</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13:H22">
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
-      <formula>$D$9="no sample"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
@@ -5289,21 +5279,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:I8"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.140625" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" customWidth="1"/>
     <col min="13" max="13" width="5.42578125" customWidth="1"/>
@@ -5326,189 +5310,189 @@
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="154" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="146"/>
-      <c r="J2" s="146"/>
-      <c r="K2" s="146"/>
-      <c r="L2" s="147"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="155"/>
+      <c r="K2" s="155"/>
+      <c r="L2" s="156"/>
       <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
-      <c r="B3" s="148"/>
-      <c r="C3" s="149"/>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149"/>
-      <c r="F3" s="149"/>
-      <c r="G3" s="149"/>
-      <c r="H3" s="149"/>
-      <c r="I3" s="149"/>
-      <c r="J3" s="149"/>
-      <c r="K3" s="149"/>
-      <c r="L3" s="150"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
+      <c r="L3" s="159"/>
       <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="164"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="165"/>
-      <c r="H4" s="165"/>
-      <c r="I4" s="165"/>
-      <c r="J4" s="99" t="s">
-        <v>75</v>
-      </c>
-      <c r="K4" s="100"/>
-      <c r="L4" s="101"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="174"/>
+      <c r="E4" s="174"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="174"/>
+      <c r="H4" s="174"/>
+      <c r="I4" s="174"/>
+      <c r="J4" s="102" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="103"/>
+      <c r="L4" s="104"/>
       <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="166"/>
-      <c r="E5" s="166"/>
-      <c r="F5" s="166"/>
-      <c r="G5" s="166"/>
-      <c r="H5" s="166"/>
-      <c r="I5" s="166"/>
-      <c r="J5" s="151" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="152"/>
-      <c r="L5" s="153"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="175"/>
+      <c r="E5" s="175"/>
+      <c r="F5" s="175"/>
+      <c r="G5" s="175"/>
+      <c r="H5" s="175"/>
+      <c r="I5" s="175"/>
+      <c r="J5" s="160" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="161"/>
+      <c r="L5" s="162"/>
       <c r="M5" s="15"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="123" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="167"/>
-      <c r="E6" s="167"/>
-      <c r="F6" s="167"/>
-      <c r="G6" s="167"/>
-      <c r="H6" s="167"/>
-      <c r="I6" s="167"/>
-      <c r="J6" s="154" t="s">
-        <v>62</v>
-      </c>
-      <c r="K6" s="155"/>
-      <c r="L6" s="156"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="176"/>
+      <c r="H6" s="176"/>
+      <c r="I6" s="176"/>
+      <c r="J6" s="163" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="164"/>
+      <c r="L6" s="165"/>
       <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="111" t="s">
+      <c r="B7" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="112"/>
-      <c r="D7" s="172"/>
-      <c r="E7" s="172"/>
-      <c r="F7" s="172"/>
-      <c r="G7" s="172"/>
-      <c r="H7" s="172"/>
-      <c r="I7" s="172"/>
-      <c r="J7" s="157" t="s">
-        <v>79</v>
-      </c>
-      <c r="K7" s="158"/>
-      <c r="L7" s="159"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="166" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="167"/>
+      <c r="L7" s="168"/>
       <c r="M7" s="15"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="111" t="s">
+      <c r="B8" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="112"/>
-      <c r="D8" s="171"/>
-      <c r="E8" s="171"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="171"/>
-      <c r="H8" s="171"/>
-      <c r="I8" s="171"/>
-      <c r="J8" s="168" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" s="169"/>
-      <c r="L8" s="170"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="180"/>
+      <c r="G8" s="180"/>
+      <c r="H8" s="180"/>
+      <c r="I8" s="180"/>
+      <c r="J8" s="177" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" s="178"/>
+      <c r="L8" s="179"/>
       <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="112"/>
-      <c r="D9" s="119" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="160" t="s">
+      <c r="C9" s="124"/>
+      <c r="D9" s="125" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="126"/>
+      <c r="J9" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="161"/>
-      <c r="L9" s="162"/>
+      <c r="K9" s="170"/>
+      <c r="L9" s="171"/>
       <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="111" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="121" t="s">
+      <c r="B10" s="123" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="124"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="122"/>
-      <c r="L10" s="123"/>
+      <c r="K10" s="128"/>
+      <c r="L10" s="129"/>
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
-      <c r="B11" s="127" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="128"/>
-      <c r="D11" s="173"/>
-      <c r="E11" s="173"/>
-      <c r="F11" s="173"/>
-      <c r="G11" s="173"/>
-      <c r="H11" s="173"/>
-      <c r="I11" s="173"/>
-      <c r="J11" s="124" t="s">
+      <c r="B11" s="133" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="134"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="181"/>
+      <c r="F11" s="181"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="181"/>
+      <c r="I11" s="181"/>
+      <c r="J11" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="125"/>
-      <c r="L11" s="126"/>
+      <c r="K11" s="131"/>
+      <c r="L11" s="132"/>
       <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:19" ht="63" x14ac:dyDescent="0.25">
@@ -5519,19 +5503,19 @@
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>6</v>
@@ -5540,18 +5524,18 @@
         <v>29</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K12" s="26" t="s">
         <v>9</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M12" s="15"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="44">
+      <c r="A13" s="43">
         <v>1</v>
       </c>
       <c r="B13" s="29"/>
@@ -5567,17 +5551,17 @@
         <f t="shared" ref="H13:H22" si="0">IFERROR(IF($D$9="standard", (G13/C13)*100, ""), "")</f>
         <v/>
       </c>
-      <c r="I13" s="45" t="str">
+      <c r="I13" s="44" t="str">
         <f>IFERROR(D13/C13*100, "")</f>
         <v/>
       </c>
-      <c r="J13" s="43"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="47"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="46"/>
       <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="44">
+      <c r="A14" s="43">
         <v>2</v>
       </c>
       <c r="B14" s="29"/>
@@ -5593,17 +5577,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I14" s="45" t="str">
+      <c r="I14" s="44" t="str">
         <f t="shared" ref="I14:I22" si="2">IFERROR(D14/C14*100, "")</f>
         <v/>
       </c>
-      <c r="J14" s="48"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="49"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="48"/>
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="44">
+      <c r="A15" s="43">
         <v>3</v>
       </c>
       <c r="B15" s="29"/>
@@ -5619,17 +5603,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I15" s="45" t="str">
+      <c r="I15" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J15" s="43"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="49"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="48"/>
       <c r="M15" s="16"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="44">
+      <c r="A16" s="43">
         <v>4</v>
       </c>
       <c r="B16" s="29"/>
@@ -5645,18 +5629,18 @@
         <f>IFERROR(IF($D$9="standard", (G16/C16)*100, ""), "")</f>
         <v/>
       </c>
-      <c r="I16" s="45" t="str">
+      <c r="I16" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J16" s="43"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="49"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="48"/>
       <c r="M16" s="15"/>
       <c r="S16" s="2"/>
     </row>
     <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="44">
+      <c r="A17" s="43">
         <v>5</v>
       </c>
       <c r="B17" s="29"/>
@@ -5672,17 +5656,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I17" s="45" t="str">
+      <c r="I17" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J17" s="43"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="49"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="48"/>
       <c r="M17" s="15"/>
     </row>
     <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
+      <c r="A18" s="43">
         <v>6</v>
       </c>
       <c r="B18" s="29"/>
@@ -5698,17 +5682,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I18" s="45" t="str">
+      <c r="I18" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J18" s="43"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="49"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="48"/>
       <c r="M18" s="15"/>
     </row>
     <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="44">
+      <c r="A19" s="43">
         <v>7</v>
       </c>
       <c r="B19" s="29"/>
@@ -5724,17 +5708,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I19" s="45" t="str">
+      <c r="I19" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J19" s="43"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="49"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="48"/>
       <c r="M19" s="15"/>
     </row>
     <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="44">
+      <c r="A20" s="43">
         <v>8</v>
       </c>
       <c r="B20" s="29"/>
@@ -5750,17 +5734,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I20" s="45" t="str">
+      <c r="I20" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J20" s="43"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="49"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="48"/>
       <c r="M20" s="15"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="44">
+      <c r="A21" s="43">
         <v>9</v>
       </c>
       <c r="B21" s="29"/>
@@ -5776,17 +5760,17 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I21" s="45" t="str">
+      <c r="I21" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J21" s="43"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="49"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="48"/>
       <c r="M21" s="15"/>
     </row>
     <row r="22" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="54">
+      <c r="A22" s="53">
         <v>10</v>
       </c>
       <c r="B22" s="29"/>
@@ -5802,89 +5786,89 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I22" s="45" t="str">
+      <c r="I22" s="44" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J22" s="33"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="51"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="50"/>
       <c r="M22" s="15"/>
     </row>
     <row r="23" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="60"/>
-      <c r="B23" s="52" t="s">
+      <c r="A23" s="59"/>
+      <c r="B23" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35" t="str">
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34" t="str">
         <f>IF(OR(ISBLANK(E23),ISBLANK(F23)),"",IF($D$9="bulk",F23-E23,""))</f>
         <v/>
       </c>
-      <c r="H23" s="36" t="str">
+      <c r="H23" s="35" t="str">
         <f>IFERROR(IF($D$9="bulk", G23/(SUM(C13:C22))*100, ""), "")</f>
         <v/>
       </c>
       <c r="I23" s="22"/>
       <c r="J23" s="22"/>
-      <c r="K23" s="129" t="s">
-        <v>61</v>
-      </c>
-      <c r="L23" s="131"/>
+      <c r="K23" s="135" t="s">
+        <v>58</v>
+      </c>
+      <c r="L23" s="137"/>
       <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="60"/>
-      <c r="B24" s="53" t="s">
+      <c r="A24" s="59"/>
+      <c r="B24" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="37">
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="36" t="str">
         <f>IF($D$9="standard",SUMIFS(G13:G22, K13:K22, ""), "")</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="39"/>
+        <v/>
+      </c>
+      <c r="H24" s="38"/>
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
-      <c r="K24" s="130"/>
-      <c r="L24" s="132"/>
+      <c r="K24" s="136"/>
+      <c r="L24" s="138"/>
       <c r="M24" s="15"/>
     </row>
     <row r="25" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="60"/>
-      <c r="B25" s="54" t="s">
+      <c r="A25" s="59"/>
+      <c r="B25" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="40" t="str">
+      <c r="C25" s="39" t="str">
         <f>IFERROR(AVERAGEIFS(C13:C22, K13:K22, ""), "")</f>
         <v/>
       </c>
-      <c r="D25" s="40" t="str">
+      <c r="D25" s="39" t="str">
         <f>IFERROR(AVERAGEIFS(D13:D22, K13:K22, ""), "")</f>
         <v/>
       </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="40" t="str">
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="39" t="str">
         <f>IFERROR(IF($D$9="Standard", AVERAGEIFS(G13:G22, K13:K22, ""), IF(D9="Bulk",G23/COUNT(D13:D22),"")),"")</f>
         <v/>
       </c>
-      <c r="H25" s="42" t="str">
+      <c r="H25" s="41" t="str">
         <f>IFERROR(IF($D$9="standard", AVERAGEIFS(H13:H22, K13:K22, ""), IF($D$9="Bulk",H23,"")), "")</f>
         <v/>
       </c>
       <c r="I25" s="22"/>
       <c r="J25" s="22"/>
-      <c r="K25" s="55" t="s">
+      <c r="K25" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="L25" s="56"/>
+      <c r="L25" s="55"/>
       <c r="M25" s="17"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
@@ -5914,16 +5898,16 @@
     </row>
     <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
-      <c r="B27" s="86" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="88"/>
+      <c r="B27" s="105" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="106"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="107"/>
       <c r="J27" s="17"/>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
@@ -5936,15 +5920,15 @@
     </row>
     <row r="28" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
-      <c r="B28" s="138" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="139"/>
-      <c r="D28" s="139"/>
-      <c r="E28" s="139"/>
-      <c r="F28" s="139"/>
-      <c r="G28" s="139"/>
-      <c r="H28" s="140"/>
+      <c r="B28" s="145" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="147"/>
       <c r="I28" s="28"/>
       <c r="J28" s="17"/>
       <c r="K28" s="15"/>
@@ -5958,19 +5942,19 @@
     </row>
     <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="63" t="s">
+      <c r="C29" s="61"/>
+      <c r="D29" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63" t="s">
+      <c r="E29" s="61"/>
+      <c r="F29" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="62"/>
-      <c r="H29" s="63" t="s">
+      <c r="G29" s="61"/>
+      <c r="H29" s="62" t="s">
         <v>16</v>
       </c>
       <c r="I29" s="28"/>
@@ -5986,22 +5970,22 @@
     </row>
     <row r="30" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15"/>
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="66" t="s">
+      <c r="C30" s="64"/>
+      <c r="D30" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="66" t="s">
+      <c r="E30" s="64"/>
+      <c r="F30" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="65"/>
-      <c r="H30" s="66" t="s">
+      <c r="G30" s="64"/>
+      <c r="H30" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="67"/>
+      <c r="I30" s="66"/>
       <c r="J30" s="17"/>
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
@@ -6014,16 +5998,16 @@
     </row>
     <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
-      <c r="B31" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="87"/>
-      <c r="I31" s="88"/>
+      <c r="B31" s="105" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="106"/>
+      <c r="I31" s="107"/>
       <c r="J31" s="17"/>
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
@@ -6036,15 +6020,15 @@
     </row>
     <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
-      <c r="B32" s="113" t="s">
+      <c r="B32" s="117" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="114"/>
-      <c r="D32" s="114"/>
-      <c r="E32" s="114"/>
-      <c r="F32" s="114"/>
-      <c r="G32" s="114"/>
-      <c r="H32" s="115"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="118"/>
+      <c r="H32" s="119"/>
       <c r="I32" s="28"/>
       <c r="J32" s="17"/>
       <c r="K32" s="17"/>
@@ -6058,15 +6042,15 @@
     </row>
     <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
-      <c r="B33" s="113" t="s">
+      <c r="B33" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="114"/>
-      <c r="D33" s="114"/>
-      <c r="E33" s="114"/>
-      <c r="F33" s="114"/>
-      <c r="G33" s="114"/>
-      <c r="H33" s="115"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="119"/>
       <c r="I33" s="28"/>
       <c r="J33" s="17"/>
       <c r="K33" s="17"/>
@@ -6080,15 +6064,15 @@
     </row>
     <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
-      <c r="B34" s="113" t="s">
+      <c r="B34" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="114"/>
-      <c r="D34" s="114"/>
-      <c r="E34" s="114"/>
-      <c r="F34" s="114"/>
-      <c r="G34" s="114"/>
-      <c r="H34" s="115"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="119"/>
       <c r="I34" s="28"/>
       <c r="J34" s="17"/>
       <c r="K34" s="17"/>
@@ -6102,15 +6086,15 @@
     </row>
     <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
-      <c r="B35" s="113" t="s">
+      <c r="B35" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="114"/>
-      <c r="D35" s="114"/>
-      <c r="E35" s="114"/>
-      <c r="F35" s="114"/>
-      <c r="G35" s="114"/>
-      <c r="H35" s="115"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="119"/>
       <c r="I35" s="28"/>
       <c r="J35" s="17"/>
       <c r="K35" s="17"/>
@@ -6124,17 +6108,17 @@
     </row>
     <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="116" t="s">
+      <c r="B36" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="117"/>
-      <c r="D36" s="117"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="118" t="s">
+      <c r="C36" s="121"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="114"/>
-      <c r="H36" s="115"/>
+      <c r="G36" s="118"/>
+      <c r="H36" s="119"/>
       <c r="I36" s="28"/>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
@@ -6148,18 +6132,18 @@
     </row>
     <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
-      <c r="B37" s="136" t="s">
+      <c r="B37" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="137"/>
-      <c r="D37" s="137"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="137" t="s">
+      <c r="C37" s="144"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="144" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="137"/>
-      <c r="H37" s="137"/>
-      <c r="I37" s="69"/>
+      <c r="G37" s="144"/>
+      <c r="H37" s="144"/>
+      <c r="I37" s="68"/>
       <c r="J37" s="17"/>
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
@@ -6172,18 +6156,18 @@
     </row>
     <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
-      <c r="B38" s="136" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="137"/>
-      <c r="D38" s="137"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="141" t="s">
-        <v>85</v>
-      </c>
-      <c r="G38" s="89"/>
-      <c r="H38" s="80"/>
-      <c r="I38" s="71"/>
+      <c r="B38" s="143" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="144"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="148" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38" s="149"/>
+      <c r="H38" s="82"/>
+      <c r="I38" s="70"/>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
       <c r="L38" s="17"/>
@@ -6196,16 +6180,16 @@
     </row>
     <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
-      <c r="B39" s="108" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" s="109"/>
-      <c r="D39" s="109"/>
-      <c r="E39" s="109"/>
-      <c r="F39" s="109"/>
-      <c r="G39" s="109"/>
-      <c r="H39" s="109"/>
-      <c r="I39" s="110"/>
+      <c r="B39" s="114" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="115"/>
+      <c r="D39" s="115"/>
+      <c r="E39" s="115"/>
+      <c r="F39" s="115"/>
+      <c r="G39" s="115"/>
+      <c r="H39" s="115"/>
+      <c r="I39" s="116"/>
       <c r="J39" s="17"/>
       <c r="K39" s="17"/>
       <c r="L39" s="17"/>
@@ -6218,14 +6202,14 @@
     </row>
     <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
-      <c r="B40" s="102"/>
-      <c r="C40" s="103"/>
-      <c r="D40" s="103"/>
-      <c r="E40" s="103"/>
-      <c r="F40" s="103"/>
-      <c r="G40" s="103"/>
-      <c r="H40" s="103"/>
-      <c r="I40" s="104"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="109"/>
+      <c r="E40" s="109"/>
+      <c r="F40" s="109"/>
+      <c r="G40" s="109"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="110"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
@@ -6238,14 +6222,14 @@
     </row>
     <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
-      <c r="B41" s="102"/>
-      <c r="C41" s="103"/>
-      <c r="D41" s="103"/>
-      <c r="E41" s="103"/>
-      <c r="F41" s="103"/>
-      <c r="G41" s="103"/>
-      <c r="H41" s="103"/>
-      <c r="I41" s="104"/>
+      <c r="B41" s="108"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="109"/>
+      <c r="F41" s="109"/>
+      <c r="G41" s="109"/>
+      <c r="H41" s="109"/>
+      <c r="I41" s="110"/>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
       <c r="L41" s="17"/>
@@ -6258,14 +6242,14 @@
     </row>
     <row r="42" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
-      <c r="B42" s="105"/>
-      <c r="C42" s="106"/>
-      <c r="D42" s="106"/>
-      <c r="E42" s="106"/>
-      <c r="F42" s="106"/>
-      <c r="G42" s="106"/>
-      <c r="H42" s="106"/>
-      <c r="I42" s="107"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="112"/>
+      <c r="G42" s="112"/>
+      <c r="H42" s="112"/>
+      <c r="I42" s="113"/>
       <c r="J42" s="17"/>
       <c r="K42" s="17"/>
       <c r="L42" s="17"/>
@@ -6278,16 +6262,16 @@
     </row>
     <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
-      <c r="B43" s="142" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="143"/>
-      <c r="D43" s="143"/>
-      <c r="E43" s="143"/>
-      <c r="F43" s="143"/>
-      <c r="G43" s="143"/>
-      <c r="H43" s="143"/>
-      <c r="I43" s="144"/>
+      <c r="B43" s="150" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="151"/>
+      <c r="D43" s="151"/>
+      <c r="E43" s="151"/>
+      <c r="F43" s="151"/>
+      <c r="G43" s="151"/>
+      <c r="H43" s="151"/>
+      <c r="I43" s="152"/>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
@@ -6300,15 +6284,15 @@
     </row>
     <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
-      <c r="B44" s="113" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="114"/>
-      <c r="D44" s="114"/>
-      <c r="E44" s="114"/>
-      <c r="F44" s="114"/>
-      <c r="G44" s="114"/>
-      <c r="H44" s="115"/>
+      <c r="B44" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="118"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="118"/>
+      <c r="F44" s="118"/>
+      <c r="G44" s="118"/>
+      <c r="H44" s="119"/>
       <c r="I44" s="28"/>
       <c r="J44" s="17"/>
       <c r="K44" s="17"/>
@@ -6322,15 +6306,15 @@
     </row>
     <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
-      <c r="B45" s="113" t="s">
+      <c r="B45" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="114"/>
-      <c r="D45" s="114"/>
-      <c r="E45" s="114"/>
-      <c r="F45" s="114"/>
-      <c r="G45" s="114"/>
-      <c r="H45" s="115"/>
+      <c r="C45" s="118"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="118"/>
+      <c r="F45" s="118"/>
+      <c r="G45" s="118"/>
+      <c r="H45" s="119"/>
       <c r="I45" s="28"/>
       <c r="J45" s="17"/>
       <c r="K45" s="17"/>
@@ -6344,15 +6328,15 @@
     </row>
     <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
-      <c r="B46" s="113" t="s">
+      <c r="B46" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="114"/>
-      <c r="D46" s="114"/>
-      <c r="E46" s="114"/>
-      <c r="F46" s="114"/>
-      <c r="G46" s="114"/>
-      <c r="H46" s="115"/>
+      <c r="C46" s="118"/>
+      <c r="D46" s="118"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118"/>
+      <c r="G46" s="118"/>
+      <c r="H46" s="119"/>
       <c r="I46" s="28"/>
       <c r="J46" s="17"/>
       <c r="K46" s="17"/>
@@ -6366,16 +6350,16 @@
     </row>
     <row r="47" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15"/>
-      <c r="B47" s="133" t="s">
+      <c r="B47" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="134"/>
-      <c r="D47" s="134"/>
-      <c r="E47" s="134"/>
-      <c r="F47" s="134"/>
-      <c r="G47" s="134"/>
-      <c r="H47" s="135"/>
-      <c r="I47" s="69"/>
+      <c r="C47" s="141"/>
+      <c r="D47" s="141"/>
+      <c r="E47" s="141"/>
+      <c r="F47" s="141"/>
+      <c r="G47" s="141"/>
+      <c r="H47" s="142"/>
+      <c r="I47" s="68"/>
       <c r="J47" s="17"/>
       <c r="K47" s="17"/>
       <c r="L47" s="17"/>
@@ -6388,16 +6372,16 @@
     </row>
     <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
-      <c r="B48" s="86" t="s">
-        <v>72</v>
-      </c>
-      <c r="C48" s="87"/>
-      <c r="D48" s="87"/>
-      <c r="E48" s="87"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="87"/>
-      <c r="H48" s="87"/>
-      <c r="I48" s="88"/>
+      <c r="B48" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="106"/>
+      <c r="D48" s="106"/>
+      <c r="E48" s="106"/>
+      <c r="F48" s="106"/>
+      <c r="G48" s="106"/>
+      <c r="H48" s="106"/>
+      <c r="I48" s="107"/>
       <c r="J48" s="17"/>
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
@@ -6405,15 +6389,15 @@
     </row>
     <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
-      <c r="B49" s="84" t="s">
-        <v>73</v>
-      </c>
-      <c r="C49" s="85"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="85"/>
+      <c r="B49" s="86" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="87"/>
+      <c r="D49" s="87"/>
+      <c r="E49" s="87"/>
+      <c r="F49" s="87"/>
+      <c r="G49" s="87"/>
+      <c r="H49" s="87"/>
       <c r="I49" s="28"/>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
@@ -6422,15 +6406,15 @@
     </row>
     <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
-      <c r="B50" s="84" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="85"/>
-      <c r="D50" s="85"/>
-      <c r="E50" s="85"/>
-      <c r="F50" s="85"/>
-      <c r="G50" s="85"/>
-      <c r="H50" s="85"/>
+      <c r="B50" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="87"/>
+      <c r="D50" s="87"/>
+      <c r="E50" s="87"/>
+      <c r="F50" s="87"/>
+      <c r="G50" s="87"/>
+      <c r="H50" s="87"/>
       <c r="I50" s="28"/>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
@@ -6439,15 +6423,15 @@
     </row>
     <row r="51" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
-      <c r="B51" s="84" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="85"/>
-      <c r="D51" s="85"/>
-      <c r="E51" s="85"/>
-      <c r="F51" s="85"/>
-      <c r="G51" s="85"/>
-      <c r="H51" s="85"/>
+      <c r="B51" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="87"/>
+      <c r="D51" s="87"/>
+      <c r="E51" s="87"/>
+      <c r="F51" s="87"/>
+      <c r="G51" s="87"/>
+      <c r="H51" s="87"/>
       <c r="I51" s="28"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
@@ -6456,16 +6440,16 @@
     </row>
     <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
-      <c r="B52" s="99" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" s="100"/>
-      <c r="D52" s="100"/>
-      <c r="E52" s="100"/>
-      <c r="F52" s="100"/>
-      <c r="G52" s="100"/>
-      <c r="H52" s="100"/>
-      <c r="I52" s="101"/>
+      <c r="B52" s="102" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="103"/>
+      <c r="D52" s="103"/>
+      <c r="E52" s="103"/>
+      <c r="F52" s="103"/>
+      <c r="G52" s="103"/>
+      <c r="H52" s="103"/>
+      <c r="I52" s="104"/>
       <c r="J52" s="17"/>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
@@ -6473,14 +6457,14 @@
     </row>
     <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
-      <c r="B53" s="93"/>
-      <c r="C53" s="94"/>
-      <c r="D53" s="94"/>
-      <c r="E53" s="94"/>
-      <c r="F53" s="94"/>
-      <c r="G53" s="94"/>
-      <c r="H53" s="94"/>
-      <c r="I53" s="95"/>
+      <c r="B53" s="96"/>
+      <c r="C53" s="97"/>
+      <c r="D53" s="97"/>
+      <c r="E53" s="97"/>
+      <c r="F53" s="97"/>
+      <c r="G53" s="97"/>
+      <c r="H53" s="97"/>
+      <c r="I53" s="98"/>
       <c r="J53" s="17"/>
       <c r="K53" s="17"/>
       <c r="L53" s="17"/>
@@ -6488,14 +6472,14 @@
     </row>
     <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
-      <c r="B54" s="93"/>
-      <c r="C54" s="94"/>
-      <c r="D54" s="94"/>
-      <c r="E54" s="94"/>
-      <c r="F54" s="94"/>
-      <c r="G54" s="94"/>
-      <c r="H54" s="94"/>
-      <c r="I54" s="95"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="97"/>
+      <c r="D54" s="97"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="97"/>
+      <c r="G54" s="97"/>
+      <c r="H54" s="97"/>
+      <c r="I54" s="98"/>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
@@ -6503,14 +6487,14 @@
     </row>
     <row r="55" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
-      <c r="B55" s="96"/>
-      <c r="C55" s="97"/>
-      <c r="D55" s="97"/>
-      <c r="E55" s="97"/>
-      <c r="F55" s="97"/>
-      <c r="G55" s="97"/>
-      <c r="H55" s="97"/>
-      <c r="I55" s="98"/>
+      <c r="B55" s="99"/>
+      <c r="C55" s="100"/>
+      <c r="D55" s="100"/>
+      <c r="E55" s="100"/>
+      <c r="F55" s="100"/>
+      <c r="G55" s="100"/>
+      <c r="H55" s="100"/>
+      <c r="I55" s="101"/>
       <c r="J55" s="17"/>
       <c r="K55" s="17"/>
       <c r="L55" s="17"/>
@@ -6548,11 +6532,11 @@
     </row>
     <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
-      <c r="B58" s="86" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="87"/>
-      <c r="D58" s="88"/>
+      <c r="B58" s="105" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" s="106"/>
+      <c r="D58" s="107"/>
       <c r="E58" s="24"/>
       <c r="F58" s="24"/>
       <c r="G58" s="24"/>
@@ -6565,11 +6549,11 @@
     </row>
     <row r="59" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="15"/>
-      <c r="B59" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="C59" s="89"/>
-      <c r="D59" s="72" t="s">
+      <c r="B59" s="81" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59" s="149"/>
+      <c r="D59" s="71" t="s">
         <v>39</v>
       </c>
       <c r="E59" s="24"/>
@@ -6584,11 +6568,11 @@
     </row>
     <row r="60" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
-      <c r="B60" s="90" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" s="91"/>
-      <c r="D60" s="73" t="s">
+      <c r="B60" s="94" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" s="153"/>
+      <c r="D60" s="72" t="s">
         <v>38</v>
       </c>
       <c r="E60" s="24"/>
@@ -6603,11 +6587,11 @@
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
-      <c r="B61" s="79" t="s">
-        <v>65</v>
-      </c>
-      <c r="C61" s="80"/>
-      <c r="D61" s="74">
+      <c r="B61" s="81" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="82"/>
+      <c r="D61" s="73">
         <v>4</v>
       </c>
       <c r="E61" s="24"/>
@@ -6622,11 +6606,11 @@
     </row>
     <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="15"/>
-      <c r="B62" s="90" t="s">
-        <v>66</v>
-      </c>
-      <c r="C62" s="92"/>
-      <c r="D62" s="73">
+      <c r="B62" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" s="95"/>
+      <c r="D62" s="72">
         <v>5</v>
       </c>
       <c r="E62" s="24"/>
@@ -6641,11 +6625,11 @@
     </row>
     <row r="63" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
-      <c r="B63" s="79" t="s">
-        <v>67</v>
-      </c>
-      <c r="C63" s="80"/>
-      <c r="D63" s="72">
+      <c r="B63" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" s="82"/>
+      <c r="D63" s="71">
         <v>50</v>
       </c>
       <c r="E63" s="24"/>
@@ -6660,11 +6644,11 @@
     </row>
     <row r="64" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="15"/>
-      <c r="B64" s="82" t="s">
-        <v>68</v>
-      </c>
-      <c r="C64" s="83"/>
-      <c r="D64" s="75">
+      <c r="B64" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="85"/>
+      <c r="D64" s="74">
         <v>66</v>
       </c>
       <c r="E64" s="24"/>
@@ -6762,7 +6746,6 @@
       <c r="B78" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zBBF0Z6GSW0g2pYctVQclDcfJIbvagbGbWtBjy60taicOVcwmpHv2ci9JA5dRpkh0Oge0XTeW3nHhEOtpKAO7Q==" saltValue="BD8J6NW8jHKgwDz/tOu8jg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="60">
     <mergeCell ref="B2:L3"/>
     <mergeCell ref="B4:C4"/>
@@ -6826,102 +6809,102 @@
     <mergeCell ref="B60:C60"/>
   </mergeCells>
   <conditionalFormatting sqref="C23:H23">
-    <cfRule type="expression" dxfId="66" priority="455">
+    <cfRule type="expression" dxfId="42" priority="455">
       <formula>$D$9="standard"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="65" priority="440">
+    <cfRule type="expression" dxfId="41" priority="440">
       <formula>D11 &lt; D10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:I7">
-    <cfRule type="expression" dxfId="64" priority="452">
+    <cfRule type="expression" dxfId="40" priority="452">
       <formula>ISBLANK($D$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="453">
+    <cfRule type="expression" dxfId="39" priority="453">
       <formula>OR(D7 &gt; D6 + 6, D7 &lt; D6 - 6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:I11">
-    <cfRule type="expression" dxfId="62" priority="439">
+    <cfRule type="expression" dxfId="38" priority="439">
       <formula>ISBLANK(D11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:F23">
-    <cfRule type="expression" dxfId="61" priority="456">
+    <cfRule type="expression" dxfId="37" priority="456">
       <formula>$D$9="bulk"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13:H22">
-    <cfRule type="expression" dxfId="60" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="1" stopIfTrue="1">
       <formula>$D$9="bulk"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13:I22 B13:D22">
-    <cfRule type="expression" dxfId="59" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="4" stopIfTrue="1">
       <formula>NOT(ISBLANK($K13))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:G22">
-    <cfRule type="cellIs" dxfId="58" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="12" operator="greaterThan">
       <formula>($H$25+$D$62)*$C13/100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="13" operator="lessThan">
       <formula>($H$25-$D$62)*$C13/100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="14" operator="greaterThanOrEqual">
       <formula>($H$25+$D$61)*$C13/100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
-    <cfRule type="expression" dxfId="55" priority="454">
+    <cfRule type="expression" dxfId="31" priority="454">
       <formula>$D$9="standard"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:H22">
-    <cfRule type="expression" dxfId="54" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="3" stopIfTrue="1">
       <formula>ISBLANK($F13)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:H23">
-    <cfRule type="expression" dxfId="53" priority="438">
+    <cfRule type="expression" dxfId="29" priority="438">
       <formula>$D$9="bulk"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:I22">
-    <cfRule type="expression" dxfId="52" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="2" stopIfTrue="1">
       <formula>ISBLANK($C13)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H22">
-    <cfRule type="cellIs" dxfId="51" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="lessThan">
       <formula>$H$25-$D$62</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="greaterThan">
       <formula>$H$25+$D$62</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="greaterThanOrEqual">
       <formula>$H$25+$D$61</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="lessThanOrEqual">
       <formula>$H$25-$D$61</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="15" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="15" operator="lessThanOrEqual">
       <formula>($H$25-$D$61)*$C13/100</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="46" priority="16">
+    <cfRule type="containsBlanks" dxfId="22" priority="16">
       <formula>LEN(TRIM(H13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:I22">
-    <cfRule type="cellIs" dxfId="45" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="greaterThan">
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="lessThan">
       <formula>$D$63</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="lessThan">
       <formula>$D$64</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6993,10 +6976,10 @@
         <v>5</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>47</v>
@@ -7008,10 +6991,10 @@
         <v>49</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -7393,97 +7376,97 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="GAGG2Sqsp8YG2XvKTukeDkEeaGM6yd0qYH11fyVXzNMHNyguqk3yd5J8DgzUdx8Jp8ocemg2K5tLzNH9CBJ7Ug==" saltValue="WpwHXy8mQW5gzr8vbbAv0w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="A3:K3">
-    <cfRule type="expression" dxfId="42" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>$K$3="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:K4">
-    <cfRule type="expression" dxfId="41" priority="18">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>$K$4="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:K5">
-    <cfRule type="expression" dxfId="40" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>$K$5="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:K6">
-    <cfRule type="expression" dxfId="39" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>$K$6="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:K7">
-    <cfRule type="expression" dxfId="38" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>$K$7="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:K8">
-    <cfRule type="expression" dxfId="37" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>$K$8="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:K9">
-    <cfRule type="expression" dxfId="36" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>$K$9="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:K10">
-    <cfRule type="expression" dxfId="35" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>$K$10="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:K11">
-    <cfRule type="expression" dxfId="34" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$K$11="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:K12">
-    <cfRule type="expression" dxfId="33" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$K$12="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:K13">
-    <cfRule type="expression" dxfId="32" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$K$13="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:K14">
-    <cfRule type="expression" dxfId="31" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$K$14="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:K15">
-    <cfRule type="expression" dxfId="30" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$K$15="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:K16">
-    <cfRule type="expression" dxfId="29" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$K$16="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:K17">
-    <cfRule type="expression" dxfId="28" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$K$17="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:K18">
-    <cfRule type="expression" dxfId="27" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$K$18="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:K19">
-    <cfRule type="expression" dxfId="26" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$K$19="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:K20">
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$K$20="yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:K21">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$K$21="yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Snow Bulletin runs, yay!
</commit_message>
<xml_diff>
--- a/inst/snow_survey/SnowSurveyTemplate.xlsx
+++ b/inst/snow_survey/SnowSurveyTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\snow_survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25784D4-8474-49D2-ACA0-0EBC9EFC15AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE4F92E-B3B1-4507-9E2D-306EE8FE5C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6465" yWindow="3150" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1352,9 +1352,240 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1412,12 +1643,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1432,15 +1657,6 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1454,222 +1670,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3618,8 +3618,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3649,189 +3649,189 @@
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="154" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="85"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="155"/>
+      <c r="K2" s="155"/>
+      <c r="L2" s="156"/>
       <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="88"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
+      <c r="L3" s="159"/>
       <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="104"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="108" t="s">
+      <c r="C4" s="173"/>
+      <c r="D4" s="174"/>
+      <c r="E4" s="174"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="174"/>
+      <c r="H4" s="174"/>
+      <c r="I4" s="174"/>
+      <c r="J4" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="K4" s="109"/>
-      <c r="L4" s="110"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="104"/>
       <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="89" t="s">
+      <c r="C5" s="124"/>
+      <c r="D5" s="175"/>
+      <c r="E5" s="175"/>
+      <c r="F5" s="175"/>
+      <c r="G5" s="175"/>
+      <c r="H5" s="175"/>
+      <c r="I5" s="175"/>
+      <c r="J5" s="160" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="90"/>
-      <c r="L5" s="91"/>
+      <c r="K5" s="161"/>
+      <c r="L5" s="162"/>
       <c r="M5" s="15"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="123" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="102"/>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="107"/>
-      <c r="J6" s="92" t="s">
+      <c r="C6" s="124"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="176"/>
+      <c r="H6" s="176"/>
+      <c r="I6" s="176"/>
+      <c r="J6" s="163" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="93"/>
-      <c r="L6" s="94"/>
+      <c r="K6" s="164"/>
+      <c r="L6" s="165"/>
       <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="102"/>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="95" t="s">
+      <c r="C7" s="124"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="166" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="96"/>
-      <c r="L7" s="97"/>
+      <c r="K7" s="167"/>
+      <c r="L7" s="168"/>
       <c r="M7" s="15"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="114"/>
-      <c r="H8" s="114"/>
-      <c r="I8" s="114"/>
-      <c r="J8" s="111" t="s">
+      <c r="C8" s="124"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="180"/>
+      <c r="G8" s="180"/>
+      <c r="H8" s="180"/>
+      <c r="I8" s="180"/>
+      <c r="J8" s="177" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="112"/>
-      <c r="L8" s="113"/>
+      <c r="K8" s="178"/>
+      <c r="L8" s="179"/>
       <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="102"/>
-      <c r="D9" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="140"/>
-      <c r="F9" s="140"/>
-      <c r="G9" s="140"/>
-      <c r="H9" s="140"/>
-      <c r="I9" s="140"/>
-      <c r="J9" s="98" t="s">
+      <c r="C9" s="124"/>
+      <c r="D9" s="125" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="126"/>
+      <c r="J9" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="99"/>
-      <c r="L9" s="100"/>
+      <c r="K9" s="170"/>
+      <c r="L9" s="171"/>
       <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="123" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="153"/>
-      <c r="E10" s="153"/>
-      <c r="F10" s="153"/>
-      <c r="G10" s="153"/>
-      <c r="H10" s="153"/>
-      <c r="I10" s="153"/>
-      <c r="J10" s="141" t="s">
+      <c r="C10" s="124"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="142"/>
-      <c r="L10" s="143"/>
+      <c r="K10" s="128"/>
+      <c r="L10" s="129"/>
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
-      <c r="B11" s="147" t="s">
+      <c r="B11" s="133" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="148"/>
-      <c r="D11" s="153"/>
-      <c r="E11" s="153"/>
-      <c r="F11" s="153"/>
-      <c r="G11" s="153"/>
-      <c r="H11" s="153"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="144" t="s">
+      <c r="C11" s="134"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="145"/>
-      <c r="L11" s="146"/>
+      <c r="K11" s="131"/>
+      <c r="L11" s="132"/>
       <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
@@ -4151,10 +4151,10 @@
       </c>
       <c r="I23" s="22"/>
       <c r="J23" s="22"/>
-      <c r="K23" s="149" t="s">
+      <c r="K23" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="L23" s="151"/>
+      <c r="L23" s="137"/>
       <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -4166,15 +4166,15 @@
       <c r="D24" s="36"/>
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
-      <c r="G24" s="36" t="str">
+      <c r="G24" s="36">
         <f>IF($D$9="standard",SUMIFS(G13:G22, K13:K22, ""), "")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H24" s="38"/>
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
-      <c r="K24" s="150"/>
-      <c r="L24" s="152"/>
+      <c r="K24" s="136"/>
+      <c r="L24" s="138"/>
       <c r="M24" s="15"/>
     </row>
     <row r="25" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4235,16 +4235,16 @@
     </row>
     <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
-      <c r="B27" s="130" t="s">
+      <c r="B27" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="131"/>
-      <c r="D27" s="131"/>
-      <c r="E27" s="131"/>
-      <c r="F27" s="131"/>
-      <c r="G27" s="131"/>
-      <c r="H27" s="131"/>
-      <c r="I27" s="132"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="107"/>
       <c r="J27" s="22"/>
       <c r="K27" s="59"/>
       <c r="L27" s="59"/>
@@ -4257,15 +4257,15 @@
     </row>
     <row r="28" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
-      <c r="B28" s="124" t="s">
+      <c r="B28" s="145" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="125"/>
-      <c r="D28" s="125"/>
-      <c r="E28" s="125"/>
-      <c r="F28" s="125"/>
-      <c r="G28" s="125"/>
-      <c r="H28" s="126"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="147"/>
       <c r="I28" s="28"/>
       <c r="J28" s="22"/>
       <c r="K28" s="59"/>
@@ -4335,16 +4335,16 @@
     </row>
     <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
-      <c r="B31" s="130" t="s">
+      <c r="B31" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="131"/>
-      <c r="D31" s="131"/>
-      <c r="E31" s="131"/>
-      <c r="F31" s="131"/>
-      <c r="G31" s="131"/>
-      <c r="H31" s="131"/>
-      <c r="I31" s="132"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="106"/>
+      <c r="I31" s="107"/>
       <c r="J31" s="22"/>
       <c r="K31" s="59"/>
       <c r="L31" s="59"/>
@@ -4357,15 +4357,15 @@
     </row>
     <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
-      <c r="B32" s="116" t="s">
+      <c r="B32" s="117" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="117"/>
-      <c r="D32" s="117"/>
-      <c r="E32" s="117"/>
-      <c r="F32" s="117"/>
-      <c r="G32" s="117"/>
-      <c r="H32" s="118"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="118"/>
+      <c r="H32" s="119"/>
       <c r="I32" s="28"/>
       <c r="J32" s="22"/>
       <c r="K32" s="22"/>
@@ -4379,15 +4379,15 @@
     </row>
     <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
-      <c r="B33" s="116" t="s">
+      <c r="B33" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="117"/>
-      <c r="D33" s="117"/>
-      <c r="E33" s="117"/>
-      <c r="F33" s="117"/>
-      <c r="G33" s="117"/>
-      <c r="H33" s="118"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="119"/>
       <c r="I33" s="28"/>
       <c r="J33" s="22"/>
       <c r="K33" s="22"/>
@@ -4401,15 +4401,15 @@
     </row>
     <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
-      <c r="B34" s="116" t="s">
+      <c r="B34" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="117"/>
-      <c r="D34" s="117"/>
-      <c r="E34" s="117"/>
-      <c r="F34" s="117"/>
-      <c r="G34" s="117"/>
-      <c r="H34" s="118"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="119"/>
       <c r="I34" s="28"/>
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
@@ -4423,15 +4423,15 @@
     </row>
     <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
-      <c r="B35" s="116" t="s">
+      <c r="B35" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="117"/>
-      <c r="D35" s="117"/>
-      <c r="E35" s="117"/>
-      <c r="F35" s="117"/>
-      <c r="G35" s="117"/>
-      <c r="H35" s="118"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="119"/>
       <c r="I35" s="28"/>
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
@@ -4445,17 +4445,17 @@
     </row>
     <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="136" t="s">
+      <c r="B36" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="137"/>
-      <c r="D36" s="137"/>
+      <c r="C36" s="121"/>
+      <c r="D36" s="121"/>
       <c r="E36" s="61"/>
-      <c r="F36" s="138" t="s">
+      <c r="F36" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="117"/>
-      <c r="H36" s="118"/>
+      <c r="G36" s="118"/>
+      <c r="H36" s="119"/>
       <c r="I36" s="28"/>
       <c r="J36" s="22"/>
       <c r="K36" s="22"/>
@@ -4469,17 +4469,17 @@
     </row>
     <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
-      <c r="B37" s="122" t="s">
+      <c r="B37" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="123"/>
-      <c r="D37" s="123"/>
+      <c r="C37" s="144"/>
+      <c r="D37" s="144"/>
       <c r="E37" s="67"/>
-      <c r="F37" s="123" t="s">
+      <c r="F37" s="144" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="123"/>
-      <c r="H37" s="123"/>
+      <c r="G37" s="144"/>
+      <c r="H37" s="144"/>
       <c r="I37" s="68"/>
       <c r="J37" s="22"/>
       <c r="K37" s="22"/>
@@ -4493,17 +4493,17 @@
     </row>
     <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
-      <c r="B38" s="122" t="s">
+      <c r="B38" s="143" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="123"/>
-      <c r="D38" s="123"/>
+      <c r="C38" s="144"/>
+      <c r="D38" s="144"/>
       <c r="E38" s="69"/>
-      <c r="F38" s="127" t="s">
+      <c r="F38" s="148" t="s">
         <v>82</v>
       </c>
-      <c r="G38" s="128"/>
-      <c r="H38" s="129"/>
+      <c r="G38" s="149"/>
+      <c r="H38" s="82"/>
       <c r="I38" s="70"/>
       <c r="J38" s="22"/>
       <c r="K38" s="22"/>
@@ -4517,16 +4517,16 @@
     </row>
     <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
-      <c r="B39" s="178" t="s">
+      <c r="B39" s="114" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="179"/>
-      <c r="D39" s="179"/>
-      <c r="E39" s="179"/>
-      <c r="F39" s="179"/>
-      <c r="G39" s="179"/>
-      <c r="H39" s="179"/>
-      <c r="I39" s="180"/>
+      <c r="C39" s="115"/>
+      <c r="D39" s="115"/>
+      <c r="E39" s="115"/>
+      <c r="F39" s="115"/>
+      <c r="G39" s="115"/>
+      <c r="H39" s="115"/>
+      <c r="I39" s="116"/>
       <c r="J39" s="22"/>
       <c r="K39" s="22"/>
       <c r="L39" s="22"/>
@@ -4539,14 +4539,14 @@
     </row>
     <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
-      <c r="B40" s="172"/>
-      <c r="C40" s="173"/>
-      <c r="D40" s="173"/>
-      <c r="E40" s="173"/>
-      <c r="F40" s="173"/>
-      <c r="G40" s="173"/>
-      <c r="H40" s="173"/>
-      <c r="I40" s="174"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="109"/>
+      <c r="E40" s="109"/>
+      <c r="F40" s="109"/>
+      <c r="G40" s="109"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="110"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
@@ -4559,14 +4559,14 @@
     </row>
     <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
-      <c r="B41" s="172"/>
-      <c r="C41" s="173"/>
-      <c r="D41" s="173"/>
-      <c r="E41" s="173"/>
-      <c r="F41" s="173"/>
-      <c r="G41" s="173"/>
-      <c r="H41" s="173"/>
-      <c r="I41" s="174"/>
+      <c r="B41" s="108"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="109"/>
+      <c r="F41" s="109"/>
+      <c r="G41" s="109"/>
+      <c r="H41" s="109"/>
+      <c r="I41" s="110"/>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
       <c r="L41" s="17"/>
@@ -4579,14 +4579,14 @@
     </row>
     <row r="42" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
-      <c r="B42" s="175"/>
-      <c r="C42" s="176"/>
-      <c r="D42" s="176"/>
-      <c r="E42" s="176"/>
-      <c r="F42" s="176"/>
-      <c r="G42" s="176"/>
-      <c r="H42" s="176"/>
-      <c r="I42" s="177"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="112"/>
+      <c r="G42" s="112"/>
+      <c r="H42" s="112"/>
+      <c r="I42" s="113"/>
       <c r="J42" s="17"/>
       <c r="K42" s="17"/>
       <c r="L42" s="17"/>
@@ -4599,16 +4599,16 @@
     </row>
     <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
-      <c r="B43" s="133" t="s">
+      <c r="B43" s="150" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="134"/>
-      <c r="D43" s="134"/>
-      <c r="E43" s="134"/>
-      <c r="F43" s="134"/>
-      <c r="G43" s="134"/>
-      <c r="H43" s="134"/>
-      <c r="I43" s="135"/>
+      <c r="C43" s="151"/>
+      <c r="D43" s="151"/>
+      <c r="E43" s="151"/>
+      <c r="F43" s="151"/>
+      <c r="G43" s="151"/>
+      <c r="H43" s="151"/>
+      <c r="I43" s="152"/>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
@@ -4621,15 +4621,15 @@
     </row>
     <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
-      <c r="B44" s="116" t="s">
+      <c r="B44" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="117"/>
-      <c r="D44" s="117"/>
-      <c r="E44" s="117"/>
-      <c r="F44" s="117"/>
-      <c r="G44" s="117"/>
-      <c r="H44" s="118"/>
+      <c r="C44" s="118"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="118"/>
+      <c r="F44" s="118"/>
+      <c r="G44" s="118"/>
+      <c r="H44" s="119"/>
       <c r="I44" s="28"/>
       <c r="J44" s="17"/>
       <c r="K44" s="17"/>
@@ -4643,15 +4643,15 @@
     </row>
     <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
-      <c r="B45" s="116" t="s">
+      <c r="B45" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="117"/>
-      <c r="D45" s="117"/>
-      <c r="E45" s="117"/>
-      <c r="F45" s="117"/>
-      <c r="G45" s="117"/>
-      <c r="H45" s="118"/>
+      <c r="C45" s="118"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="118"/>
+      <c r="F45" s="118"/>
+      <c r="G45" s="118"/>
+      <c r="H45" s="119"/>
       <c r="I45" s="28"/>
       <c r="J45" s="17"/>
       <c r="K45" s="17"/>
@@ -4665,15 +4665,15 @@
     </row>
     <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
-      <c r="B46" s="116" t="s">
+      <c r="B46" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="117"/>
-      <c r="D46" s="117"/>
-      <c r="E46" s="117"/>
-      <c r="F46" s="117"/>
-      <c r="G46" s="117"/>
-      <c r="H46" s="118"/>
+      <c r="C46" s="118"/>
+      <c r="D46" s="118"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118"/>
+      <c r="G46" s="118"/>
+      <c r="H46" s="119"/>
       <c r="I46" s="28"/>
       <c r="J46" s="17"/>
       <c r="K46" s="17"/>
@@ -4687,15 +4687,15 @@
     </row>
     <row r="47" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15"/>
-      <c r="B47" s="119" t="s">
+      <c r="B47" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="120"/>
-      <c r="D47" s="120"/>
-      <c r="E47" s="120"/>
-      <c r="F47" s="120"/>
-      <c r="G47" s="120"/>
-      <c r="H47" s="121"/>
+      <c r="C47" s="141"/>
+      <c r="D47" s="141"/>
+      <c r="E47" s="141"/>
+      <c r="F47" s="141"/>
+      <c r="G47" s="141"/>
+      <c r="H47" s="142"/>
       <c r="I47" s="68"/>
       <c r="J47" s="17"/>
       <c r="K47" s="17"/>
@@ -4709,16 +4709,16 @@
     </row>
     <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
-      <c r="B48" s="130" t="s">
+      <c r="B48" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="131"/>
-      <c r="D48" s="131"/>
-      <c r="E48" s="131"/>
-      <c r="F48" s="131"/>
-      <c r="G48" s="131"/>
-      <c r="H48" s="131"/>
-      <c r="I48" s="132"/>
+      <c r="C48" s="106"/>
+      <c r="D48" s="106"/>
+      <c r="E48" s="106"/>
+      <c r="F48" s="106"/>
+      <c r="G48" s="106"/>
+      <c r="H48" s="106"/>
+      <c r="I48" s="107"/>
       <c r="J48" s="17"/>
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
@@ -4726,15 +4726,15 @@
     </row>
     <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
-      <c r="B49" s="157" t="s">
+      <c r="B49" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="158"/>
-      <c r="D49" s="158"/>
-      <c r="E49" s="158"/>
-      <c r="F49" s="158"/>
-      <c r="G49" s="158"/>
-      <c r="H49" s="158"/>
+      <c r="C49" s="87"/>
+      <c r="D49" s="87"/>
+      <c r="E49" s="87"/>
+      <c r="F49" s="87"/>
+      <c r="G49" s="87"/>
+      <c r="H49" s="87"/>
       <c r="I49" s="28"/>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
@@ -4743,15 +4743,15 @@
     </row>
     <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
-      <c r="B50" s="157" t="s">
+      <c r="B50" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="158"/>
-      <c r="D50" s="158"/>
-      <c r="E50" s="158"/>
-      <c r="F50" s="158"/>
-      <c r="G50" s="158"/>
-      <c r="H50" s="158"/>
+      <c r="C50" s="87"/>
+      <c r="D50" s="87"/>
+      <c r="E50" s="87"/>
+      <c r="F50" s="87"/>
+      <c r="G50" s="87"/>
+      <c r="H50" s="87"/>
       <c r="I50" s="28"/>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
@@ -4760,15 +4760,15 @@
     </row>
     <row r="51" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
-      <c r="B51" s="157" t="s">
+      <c r="B51" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="158"/>
-      <c r="D51" s="158"/>
-      <c r="E51" s="158"/>
-      <c r="F51" s="158"/>
-      <c r="G51" s="158"/>
-      <c r="H51" s="158"/>
+      <c r="C51" s="87"/>
+      <c r="D51" s="87"/>
+      <c r="E51" s="87"/>
+      <c r="F51" s="87"/>
+      <c r="G51" s="87"/>
+      <c r="H51" s="87"/>
       <c r="I51" s="28"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
@@ -4777,16 +4777,16 @@
     </row>
     <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
-      <c r="B52" s="108" t="s">
+      <c r="B52" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="109"/>
-      <c r="D52" s="109"/>
-      <c r="E52" s="109"/>
-      <c r="F52" s="109"/>
-      <c r="G52" s="109"/>
-      <c r="H52" s="109"/>
-      <c r="I52" s="110"/>
+      <c r="C52" s="103"/>
+      <c r="D52" s="103"/>
+      <c r="E52" s="103"/>
+      <c r="F52" s="103"/>
+      <c r="G52" s="103"/>
+      <c r="H52" s="103"/>
+      <c r="I52" s="104"/>
       <c r="J52" s="17"/>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
@@ -4794,14 +4794,14 @@
     </row>
     <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
-      <c r="B53" s="166"/>
-      <c r="C53" s="167"/>
-      <c r="D53" s="167"/>
-      <c r="E53" s="167"/>
-      <c r="F53" s="167"/>
-      <c r="G53" s="167"/>
-      <c r="H53" s="167"/>
-      <c r="I53" s="168"/>
+      <c r="B53" s="96"/>
+      <c r="C53" s="97"/>
+      <c r="D53" s="97"/>
+      <c r="E53" s="97"/>
+      <c r="F53" s="97"/>
+      <c r="G53" s="97"/>
+      <c r="H53" s="97"/>
+      <c r="I53" s="98"/>
       <c r="J53" s="17"/>
       <c r="K53" s="17"/>
       <c r="L53" s="17"/>
@@ -4809,14 +4809,14 @@
     </row>
     <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
-      <c r="B54" s="166"/>
-      <c r="C54" s="167"/>
-      <c r="D54" s="167"/>
-      <c r="E54" s="167"/>
-      <c r="F54" s="167"/>
-      <c r="G54" s="167"/>
-      <c r="H54" s="167"/>
-      <c r="I54" s="168"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="97"/>
+      <c r="D54" s="97"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="97"/>
+      <c r="G54" s="97"/>
+      <c r="H54" s="97"/>
+      <c r="I54" s="98"/>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
@@ -4824,14 +4824,14 @@
     </row>
     <row r="55" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
-      <c r="B55" s="169"/>
-      <c r="C55" s="170"/>
-      <c r="D55" s="170"/>
-      <c r="E55" s="170"/>
-      <c r="F55" s="170"/>
-      <c r="G55" s="170"/>
-      <c r="H55" s="170"/>
-      <c r="I55" s="171"/>
+      <c r="B55" s="99"/>
+      <c r="C55" s="100"/>
+      <c r="D55" s="100"/>
+      <c r="E55" s="100"/>
+      <c r="F55" s="100"/>
+      <c r="G55" s="100"/>
+      <c r="H55" s="100"/>
+      <c r="I55" s="101"/>
       <c r="J55" s="17"/>
       <c r="K55" s="17"/>
       <c r="L55" s="17"/>
@@ -4854,11 +4854,11 @@
     </row>
     <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
-      <c r="B57" s="159" t="s">
+      <c r="B57" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="C57" s="160"/>
-      <c r="D57" s="161"/>
+      <c r="C57" s="89"/>
+      <c r="D57" s="90"/>
       <c r="E57" s="24"/>
       <c r="F57" s="24"/>
       <c r="G57" s="24"/>
@@ -4890,10 +4890,10 @@
     </row>
     <row r="59" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="15"/>
-      <c r="B59" s="162" t="s">
+      <c r="B59" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="C59" s="163"/>
+      <c r="C59" s="92"/>
       <c r="D59" s="79" t="s">
         <v>38</v>
       </c>
@@ -4909,10 +4909,10 @@
     </row>
     <row r="60" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
-      <c r="B60" s="81" t="s">
+      <c r="B60" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="82"/>
+      <c r="C60" s="153"/>
       <c r="D60" s="80" t="s">
         <v>86</v>
       </c>
@@ -4928,10 +4928,10 @@
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
-      <c r="B61" s="162" t="s">
+      <c r="B61" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="C61" s="164"/>
+      <c r="C61" s="93"/>
       <c r="D61" s="73">
         <v>4</v>
       </c>
@@ -4947,10 +4947,10 @@
     </row>
     <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="15"/>
-      <c r="B62" s="81" t="s">
+      <c r="B62" s="94" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="165"/>
+      <c r="C62" s="95"/>
       <c r="D62" s="72">
         <v>5</v>
       </c>
@@ -4966,10 +4966,10 @@
     </row>
     <row r="63" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
-      <c r="B63" s="154" t="s">
+      <c r="B63" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="129"/>
+      <c r="C63" s="82"/>
       <c r="D63" s="71">
         <v>50</v>
       </c>
@@ -4985,10 +4985,10 @@
     </row>
     <row r="64" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="15"/>
-      <c r="B64" s="155" t="s">
+      <c r="B64" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="156"/>
+      <c r="C64" s="85"/>
       <c r="D64" s="74">
         <v>66</v>
       </c>
@@ -5089,6 +5089,50 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="JlmkU2A/qCOqNtuxGXe+SVKYclyFs2igpOrvqEJgmC1cSq3wMFELsRLHn11yJqGHqT8B8B9tnhZ8vbhMRFGlaA==" saltValue="2am05ntsdCUtj9sTWLXQEw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="60">
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="D10:I10"/>
     <mergeCell ref="B64:C64"/>
@@ -5105,50 +5149,6 @@
     <mergeCell ref="B40:I42"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B2:L3"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="D8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="C13:H22">
     <cfRule type="expression" dxfId="66" priority="2" stopIfTrue="1">
@@ -5280,8 +5280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5311,189 +5311,189 @@
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="154" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="85"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="155"/>
+      <c r="K2" s="155"/>
+      <c r="L2" s="156"/>
       <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="88"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
+      <c r="L3" s="159"/>
       <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="104"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="108" t="s">
+      <c r="C4" s="173"/>
+      <c r="D4" s="174"/>
+      <c r="E4" s="174"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="174"/>
+      <c r="H4" s="174"/>
+      <c r="I4" s="174"/>
+      <c r="J4" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="K4" s="109"/>
-      <c r="L4" s="110"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="104"/>
       <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="89" t="s">
+      <c r="C5" s="124"/>
+      <c r="D5" s="175"/>
+      <c r="E5" s="175"/>
+      <c r="F5" s="175"/>
+      <c r="G5" s="175"/>
+      <c r="H5" s="175"/>
+      <c r="I5" s="175"/>
+      <c r="J5" s="160" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="90"/>
-      <c r="L5" s="91"/>
+      <c r="K5" s="161"/>
+      <c r="L5" s="162"/>
       <c r="M5" s="15"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="123" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="102"/>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="107"/>
-      <c r="J6" s="92" t="s">
+      <c r="C6" s="124"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="176"/>
+      <c r="H6" s="176"/>
+      <c r="I6" s="176"/>
+      <c r="J6" s="163" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="93"/>
-      <c r="L6" s="94"/>
+      <c r="K6" s="164"/>
+      <c r="L6" s="165"/>
       <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="102"/>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="95" t="s">
+      <c r="C7" s="124"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="166" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="96"/>
-      <c r="L7" s="97"/>
+      <c r="K7" s="167"/>
+      <c r="L7" s="168"/>
       <c r="M7" s="15"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="114"/>
-      <c r="H8" s="114"/>
-      <c r="I8" s="114"/>
-      <c r="J8" s="111" t="s">
+      <c r="C8" s="124"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="180"/>
+      <c r="G8" s="180"/>
+      <c r="H8" s="180"/>
+      <c r="I8" s="180"/>
+      <c r="J8" s="177" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="112"/>
-      <c r="L8" s="113"/>
+      <c r="K8" s="178"/>
+      <c r="L8" s="179"/>
       <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="102"/>
-      <c r="D9" s="139" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="140"/>
-      <c r="F9" s="140"/>
-      <c r="G9" s="140"/>
-      <c r="H9" s="140"/>
-      <c r="I9" s="140"/>
-      <c r="J9" s="98" t="s">
+      <c r="C9" s="124"/>
+      <c r="D9" s="125" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="126"/>
+      <c r="J9" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="99"/>
-      <c r="L9" s="100"/>
+      <c r="K9" s="170"/>
+      <c r="L9" s="171"/>
       <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="123" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="153"/>
-      <c r="E10" s="153"/>
-      <c r="F10" s="153"/>
-      <c r="G10" s="153"/>
-      <c r="H10" s="153"/>
-      <c r="I10" s="153"/>
-      <c r="J10" s="141" t="s">
+      <c r="C10" s="124"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="142"/>
-      <c r="L10" s="143"/>
+      <c r="K10" s="128"/>
+      <c r="L10" s="129"/>
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
-      <c r="B11" s="147" t="s">
+      <c r="B11" s="133" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="148"/>
+      <c r="C11" s="134"/>
       <c r="D11" s="181"/>
       <c r="E11" s="181"/>
       <c r="F11" s="181"/>
       <c r="G11" s="181"/>
       <c r="H11" s="181"/>
       <c r="I11" s="181"/>
-      <c r="J11" s="144" t="s">
+      <c r="J11" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="145"/>
-      <c r="L11" s="146"/>
+      <c r="K11" s="131"/>
+      <c r="L11" s="132"/>
       <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:19" ht="63" x14ac:dyDescent="0.25">
@@ -5815,10 +5815,10 @@
       </c>
       <c r="I23" s="22"/>
       <c r="J23" s="22"/>
-      <c r="K23" s="149" t="s">
+      <c r="K23" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="L23" s="151"/>
+      <c r="L23" s="137"/>
       <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -5830,15 +5830,15 @@
       <c r="D24" s="36"/>
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
-      <c r="G24" s="36" t="str">
+      <c r="G24" s="36">
         <f>IF($D$9="standard",SUMIFS(G13:G22, K13:K22, ""), "")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="H24" s="38"/>
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
-      <c r="K24" s="150"/>
-      <c r="L24" s="152"/>
+      <c r="K24" s="136"/>
+      <c r="L24" s="138"/>
       <c r="M24" s="15"/>
     </row>
     <row r="25" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5899,16 +5899,16 @@
     </row>
     <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
-      <c r="B27" s="130" t="s">
+      <c r="B27" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="131"/>
-      <c r="D27" s="131"/>
-      <c r="E27" s="131"/>
-      <c r="F27" s="131"/>
-      <c r="G27" s="131"/>
-      <c r="H27" s="131"/>
-      <c r="I27" s="132"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="107"/>
       <c r="J27" s="17"/>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
@@ -5921,15 +5921,15 @@
     </row>
     <row r="28" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
-      <c r="B28" s="124" t="s">
+      <c r="B28" s="145" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="125"/>
-      <c r="D28" s="125"/>
-      <c r="E28" s="125"/>
-      <c r="F28" s="125"/>
-      <c r="G28" s="125"/>
-      <c r="H28" s="126"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="147"/>
       <c r="I28" s="28"/>
       <c r="J28" s="17"/>
       <c r="K28" s="15"/>
@@ -5999,16 +5999,16 @@
     </row>
     <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
-      <c r="B31" s="130" t="s">
+      <c r="B31" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="131"/>
-      <c r="D31" s="131"/>
-      <c r="E31" s="131"/>
-      <c r="F31" s="131"/>
-      <c r="G31" s="131"/>
-      <c r="H31" s="131"/>
-      <c r="I31" s="132"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="106"/>
+      <c r="I31" s="107"/>
       <c r="J31" s="17"/>
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
@@ -6021,15 +6021,15 @@
     </row>
     <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
-      <c r="B32" s="116" t="s">
+      <c r="B32" s="117" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="117"/>
-      <c r="D32" s="117"/>
-      <c r="E32" s="117"/>
-      <c r="F32" s="117"/>
-      <c r="G32" s="117"/>
-      <c r="H32" s="118"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="118"/>
+      <c r="H32" s="119"/>
       <c r="I32" s="28"/>
       <c r="J32" s="17"/>
       <c r="K32" s="17"/>
@@ -6043,15 +6043,15 @@
     </row>
     <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
-      <c r="B33" s="116" t="s">
+      <c r="B33" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="117"/>
-      <c r="D33" s="117"/>
-      <c r="E33" s="117"/>
-      <c r="F33" s="117"/>
-      <c r="G33" s="117"/>
-      <c r="H33" s="118"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="119"/>
       <c r="I33" s="28"/>
       <c r="J33" s="17"/>
       <c r="K33" s="17"/>
@@ -6065,15 +6065,15 @@
     </row>
     <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
-      <c r="B34" s="116" t="s">
+      <c r="B34" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="117"/>
-      <c r="D34" s="117"/>
-      <c r="E34" s="117"/>
-      <c r="F34" s="117"/>
-      <c r="G34" s="117"/>
-      <c r="H34" s="118"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="119"/>
       <c r="I34" s="28"/>
       <c r="J34" s="17"/>
       <c r="K34" s="17"/>
@@ -6087,15 +6087,15 @@
     </row>
     <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
-      <c r="B35" s="116" t="s">
+      <c r="B35" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="117"/>
-      <c r="D35" s="117"/>
-      <c r="E35" s="117"/>
-      <c r="F35" s="117"/>
-      <c r="G35" s="117"/>
-      <c r="H35" s="118"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="119"/>
       <c r="I35" s="28"/>
       <c r="J35" s="17"/>
       <c r="K35" s="17"/>
@@ -6109,17 +6109,17 @@
     </row>
     <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="136" t="s">
+      <c r="B36" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="137"/>
-      <c r="D36" s="137"/>
+      <c r="C36" s="121"/>
+      <c r="D36" s="121"/>
       <c r="E36" s="61"/>
-      <c r="F36" s="138" t="s">
+      <c r="F36" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="117"/>
-      <c r="H36" s="118"/>
+      <c r="G36" s="118"/>
+      <c r="H36" s="119"/>
       <c r="I36" s="28"/>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
@@ -6133,17 +6133,17 @@
     </row>
     <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
-      <c r="B37" s="122" t="s">
+      <c r="B37" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="123"/>
-      <c r="D37" s="123"/>
+      <c r="C37" s="144"/>
+      <c r="D37" s="144"/>
       <c r="E37" s="67"/>
-      <c r="F37" s="123" t="s">
+      <c r="F37" s="144" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="123"/>
-      <c r="H37" s="123"/>
+      <c r="G37" s="144"/>
+      <c r="H37" s="144"/>
       <c r="I37" s="68"/>
       <c r="J37" s="17"/>
       <c r="K37" s="17"/>
@@ -6157,17 +6157,17 @@
     </row>
     <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
-      <c r="B38" s="122" t="s">
+      <c r="B38" s="143" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="123"/>
-      <c r="D38" s="123"/>
+      <c r="C38" s="144"/>
+      <c r="D38" s="144"/>
       <c r="E38" s="69"/>
-      <c r="F38" s="127" t="s">
+      <c r="F38" s="148" t="s">
         <v>82</v>
       </c>
-      <c r="G38" s="128"/>
-      <c r="H38" s="129"/>
+      <c r="G38" s="149"/>
+      <c r="H38" s="82"/>
       <c r="I38" s="70"/>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
@@ -6181,16 +6181,16 @@
     </row>
     <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
-      <c r="B39" s="178" t="s">
+      <c r="B39" s="114" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="179"/>
-      <c r="D39" s="179"/>
-      <c r="E39" s="179"/>
-      <c r="F39" s="179"/>
-      <c r="G39" s="179"/>
-      <c r="H39" s="179"/>
-      <c r="I39" s="180"/>
+      <c r="C39" s="115"/>
+      <c r="D39" s="115"/>
+      <c r="E39" s="115"/>
+      <c r="F39" s="115"/>
+      <c r="G39" s="115"/>
+      <c r="H39" s="115"/>
+      <c r="I39" s="116"/>
       <c r="J39" s="17"/>
       <c r="K39" s="17"/>
       <c r="L39" s="17"/>
@@ -6203,14 +6203,14 @@
     </row>
     <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
-      <c r="B40" s="172"/>
-      <c r="C40" s="173"/>
-      <c r="D40" s="173"/>
-      <c r="E40" s="173"/>
-      <c r="F40" s="173"/>
-      <c r="G40" s="173"/>
-      <c r="H40" s="173"/>
-      <c r="I40" s="174"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="109"/>
+      <c r="E40" s="109"/>
+      <c r="F40" s="109"/>
+      <c r="G40" s="109"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="110"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
@@ -6223,14 +6223,14 @@
     </row>
     <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
-      <c r="B41" s="172"/>
-      <c r="C41" s="173"/>
-      <c r="D41" s="173"/>
-      <c r="E41" s="173"/>
-      <c r="F41" s="173"/>
-      <c r="G41" s="173"/>
-      <c r="H41" s="173"/>
-      <c r="I41" s="174"/>
+      <c r="B41" s="108"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="109"/>
+      <c r="F41" s="109"/>
+      <c r="G41" s="109"/>
+      <c r="H41" s="109"/>
+      <c r="I41" s="110"/>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
       <c r="L41" s="17"/>
@@ -6243,14 +6243,14 @@
     </row>
     <row r="42" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
-      <c r="B42" s="175"/>
-      <c r="C42" s="176"/>
-      <c r="D42" s="176"/>
-      <c r="E42" s="176"/>
-      <c r="F42" s="176"/>
-      <c r="G42" s="176"/>
-      <c r="H42" s="176"/>
-      <c r="I42" s="177"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="112"/>
+      <c r="G42" s="112"/>
+      <c r="H42" s="112"/>
+      <c r="I42" s="113"/>
       <c r="J42" s="17"/>
       <c r="K42" s="17"/>
       <c r="L42" s="17"/>
@@ -6263,16 +6263,16 @@
     </row>
     <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
-      <c r="B43" s="133" t="s">
+      <c r="B43" s="150" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="134"/>
-      <c r="D43" s="134"/>
-      <c r="E43" s="134"/>
-      <c r="F43" s="134"/>
-      <c r="G43" s="134"/>
-      <c r="H43" s="134"/>
-      <c r="I43" s="135"/>
+      <c r="C43" s="151"/>
+      <c r="D43" s="151"/>
+      <c r="E43" s="151"/>
+      <c r="F43" s="151"/>
+      <c r="G43" s="151"/>
+      <c r="H43" s="151"/>
+      <c r="I43" s="152"/>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
@@ -6285,15 +6285,15 @@
     </row>
     <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
-      <c r="B44" s="116" t="s">
+      <c r="B44" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="117"/>
-      <c r="D44" s="117"/>
-      <c r="E44" s="117"/>
-      <c r="F44" s="117"/>
-      <c r="G44" s="117"/>
-      <c r="H44" s="118"/>
+      <c r="C44" s="118"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="118"/>
+      <c r="F44" s="118"/>
+      <c r="G44" s="118"/>
+      <c r="H44" s="119"/>
       <c r="I44" s="28"/>
       <c r="J44" s="17"/>
       <c r="K44" s="17"/>
@@ -6307,15 +6307,15 @@
     </row>
     <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
-      <c r="B45" s="116" t="s">
+      <c r="B45" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="117"/>
-      <c r="D45" s="117"/>
-      <c r="E45" s="117"/>
-      <c r="F45" s="117"/>
-      <c r="G45" s="117"/>
-      <c r="H45" s="118"/>
+      <c r="C45" s="118"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="118"/>
+      <c r="F45" s="118"/>
+      <c r="G45" s="118"/>
+      <c r="H45" s="119"/>
       <c r="I45" s="28"/>
       <c r="J45" s="17"/>
       <c r="K45" s="17"/>
@@ -6329,15 +6329,15 @@
     </row>
     <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
-      <c r="B46" s="116" t="s">
+      <c r="B46" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="117"/>
-      <c r="D46" s="117"/>
-      <c r="E46" s="117"/>
-      <c r="F46" s="117"/>
-      <c r="G46" s="117"/>
-      <c r="H46" s="118"/>
+      <c r="C46" s="118"/>
+      <c r="D46" s="118"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118"/>
+      <c r="G46" s="118"/>
+      <c r="H46" s="119"/>
       <c r="I46" s="28"/>
       <c r="J46" s="17"/>
       <c r="K46" s="17"/>
@@ -6351,15 +6351,15 @@
     </row>
     <row r="47" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15"/>
-      <c r="B47" s="119" t="s">
+      <c r="B47" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="120"/>
-      <c r="D47" s="120"/>
-      <c r="E47" s="120"/>
-      <c r="F47" s="120"/>
-      <c r="G47" s="120"/>
-      <c r="H47" s="121"/>
+      <c r="C47" s="141"/>
+      <c r="D47" s="141"/>
+      <c r="E47" s="141"/>
+      <c r="F47" s="141"/>
+      <c r="G47" s="141"/>
+      <c r="H47" s="142"/>
       <c r="I47" s="68"/>
       <c r="J47" s="17"/>
       <c r="K47" s="17"/>
@@ -6373,16 +6373,16 @@
     </row>
     <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
-      <c r="B48" s="130" t="s">
+      <c r="B48" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="131"/>
-      <c r="D48" s="131"/>
-      <c r="E48" s="131"/>
-      <c r="F48" s="131"/>
-      <c r="G48" s="131"/>
-      <c r="H48" s="131"/>
-      <c r="I48" s="132"/>
+      <c r="C48" s="106"/>
+      <c r="D48" s="106"/>
+      <c r="E48" s="106"/>
+      <c r="F48" s="106"/>
+      <c r="G48" s="106"/>
+      <c r="H48" s="106"/>
+      <c r="I48" s="107"/>
       <c r="J48" s="17"/>
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
@@ -6390,15 +6390,15 @@
     </row>
     <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
-      <c r="B49" s="157" t="s">
+      <c r="B49" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="158"/>
-      <c r="D49" s="158"/>
-      <c r="E49" s="158"/>
-      <c r="F49" s="158"/>
-      <c r="G49" s="158"/>
-      <c r="H49" s="158"/>
+      <c r="C49" s="87"/>
+      <c r="D49" s="87"/>
+      <c r="E49" s="87"/>
+      <c r="F49" s="87"/>
+      <c r="G49" s="87"/>
+      <c r="H49" s="87"/>
       <c r="I49" s="28"/>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
@@ -6407,15 +6407,15 @@
     </row>
     <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
-      <c r="B50" s="157" t="s">
+      <c r="B50" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="158"/>
-      <c r="D50" s="158"/>
-      <c r="E50" s="158"/>
-      <c r="F50" s="158"/>
-      <c r="G50" s="158"/>
-      <c r="H50" s="158"/>
+      <c r="C50" s="87"/>
+      <c r="D50" s="87"/>
+      <c r="E50" s="87"/>
+      <c r="F50" s="87"/>
+      <c r="G50" s="87"/>
+      <c r="H50" s="87"/>
       <c r="I50" s="28"/>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
@@ -6424,15 +6424,15 @@
     </row>
     <row r="51" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
-      <c r="B51" s="157" t="s">
+      <c r="B51" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="158"/>
-      <c r="D51" s="158"/>
-      <c r="E51" s="158"/>
-      <c r="F51" s="158"/>
-      <c r="G51" s="158"/>
-      <c r="H51" s="158"/>
+      <c r="C51" s="87"/>
+      <c r="D51" s="87"/>
+      <c r="E51" s="87"/>
+      <c r="F51" s="87"/>
+      <c r="G51" s="87"/>
+      <c r="H51" s="87"/>
       <c r="I51" s="28"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
@@ -6441,16 +6441,16 @@
     </row>
     <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
-      <c r="B52" s="108" t="s">
+      <c r="B52" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="109"/>
-      <c r="D52" s="109"/>
-      <c r="E52" s="109"/>
-      <c r="F52" s="109"/>
-      <c r="G52" s="109"/>
-      <c r="H52" s="109"/>
-      <c r="I52" s="110"/>
+      <c r="C52" s="103"/>
+      <c r="D52" s="103"/>
+      <c r="E52" s="103"/>
+      <c r="F52" s="103"/>
+      <c r="G52" s="103"/>
+      <c r="H52" s="103"/>
+      <c r="I52" s="104"/>
       <c r="J52" s="17"/>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
@@ -6458,14 +6458,14 @@
     </row>
     <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
-      <c r="B53" s="166"/>
-      <c r="C53" s="167"/>
-      <c r="D53" s="167"/>
-      <c r="E53" s="167"/>
-      <c r="F53" s="167"/>
-      <c r="G53" s="167"/>
-      <c r="H53" s="167"/>
-      <c r="I53" s="168"/>
+      <c r="B53" s="96"/>
+      <c r="C53" s="97"/>
+      <c r="D53" s="97"/>
+      <c r="E53" s="97"/>
+      <c r="F53" s="97"/>
+      <c r="G53" s="97"/>
+      <c r="H53" s="97"/>
+      <c r="I53" s="98"/>
       <c r="J53" s="17"/>
       <c r="K53" s="17"/>
       <c r="L53" s="17"/>
@@ -6473,14 +6473,14 @@
     </row>
     <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
-      <c r="B54" s="166"/>
-      <c r="C54" s="167"/>
-      <c r="D54" s="167"/>
-      <c r="E54" s="167"/>
-      <c r="F54" s="167"/>
-      <c r="G54" s="167"/>
-      <c r="H54" s="167"/>
-      <c r="I54" s="168"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="97"/>
+      <c r="D54" s="97"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="97"/>
+      <c r="G54" s="97"/>
+      <c r="H54" s="97"/>
+      <c r="I54" s="98"/>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
@@ -6488,14 +6488,14 @@
     </row>
     <row r="55" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
-      <c r="B55" s="169"/>
-      <c r="C55" s="170"/>
-      <c r="D55" s="170"/>
-      <c r="E55" s="170"/>
-      <c r="F55" s="170"/>
-      <c r="G55" s="170"/>
-      <c r="H55" s="170"/>
-      <c r="I55" s="171"/>
+      <c r="B55" s="99"/>
+      <c r="C55" s="100"/>
+      <c r="D55" s="100"/>
+      <c r="E55" s="100"/>
+      <c r="F55" s="100"/>
+      <c r="G55" s="100"/>
+      <c r="H55" s="100"/>
+      <c r="I55" s="101"/>
       <c r="J55" s="17"/>
       <c r="K55" s="17"/>
       <c r="L55" s="17"/>
@@ -6533,11 +6533,11 @@
     </row>
     <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
-      <c r="B58" s="130" t="s">
+      <c r="B58" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="131"/>
-      <c r="D58" s="132"/>
+      <c r="C58" s="106"/>
+      <c r="D58" s="107"/>
       <c r="E58" s="24"/>
       <c r="F58" s="24"/>
       <c r="G58" s="24"/>
@@ -6550,10 +6550,10 @@
     </row>
     <row r="59" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="15"/>
-      <c r="B59" s="154" t="s">
+      <c r="B59" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="128"/>
+      <c r="C59" s="149"/>
       <c r="D59" s="71" t="s">
         <v>39</v>
       </c>
@@ -6569,10 +6569,10 @@
     </row>
     <row r="60" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
-      <c r="B60" s="81" t="s">
+      <c r="B60" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="C60" s="82"/>
+      <c r="C60" s="153"/>
       <c r="D60" s="72" t="s">
         <v>38</v>
       </c>
@@ -6588,10 +6588,10 @@
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
-      <c r="B61" s="154" t="s">
+      <c r="B61" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="C61" s="129"/>
+      <c r="C61" s="82"/>
       <c r="D61" s="73">
         <v>4</v>
       </c>
@@ -6607,10 +6607,10 @@
     </row>
     <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="15"/>
-      <c r="B62" s="81" t="s">
+      <c r="B62" s="94" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="165"/>
+      <c r="C62" s="95"/>
       <c r="D62" s="72">
         <v>5</v>
       </c>
@@ -6626,10 +6626,10 @@
     </row>
     <row r="63" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
-      <c r="B63" s="154" t="s">
+      <c r="B63" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="129"/>
+      <c r="C63" s="82"/>
       <c r="D63" s="71">
         <v>50</v>
       </c>
@@ -6645,10 +6645,10 @@
     </row>
     <row r="64" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="15"/>
-      <c r="B64" s="155" t="s">
+      <c r="B64" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="156"/>
+      <c r="C64" s="85"/>
       <c r="D64" s="74">
         <v>66</v>
       </c>
@@ -6749,28 +6749,31 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="oJxLpNuUjx9MFBlVxObjL9zXLqa74Z223FiZtLoMDG9RPIA1ZvAg5vzF9kSBuHSxVCPouGEdCaraarVN8qu93g==" saltValue="WlTY9IqluZOZyB/V3WUPtg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="60">
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B51:H51"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B53:I55"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B50:H50"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="B39:I39"/>
-    <mergeCell ref="B40:I42"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B48:I48"/>
-    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:I10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="J11:L11"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="F37:H37"/>
     <mergeCell ref="K23:K24"/>
@@ -6784,31 +6787,28 @@
     <mergeCell ref="B35:H35"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:I10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="B2:L3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B40:I42"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B53:I55"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
   </mergeCells>
   <conditionalFormatting sqref="C23:H23">
     <cfRule type="expression" dxfId="42" priority="455">

</xml_diff>